<commit_message>
Create piling _roperties.xlsx; update properties.xlsx
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8654467-3A54-7F49-AD1B-D8D7E11D058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62878DD1-CEFF-1445-920F-EA96DD1CD152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="860" windowWidth="46240" windowHeight="29160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8440" yWindow="860" windowWidth="46240" windowHeight="29160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="783">
   <si>
     <t>Description</t>
   </si>
@@ -2377,6 +2377,15 @@
   </si>
   <si>
     <t>//diggs_geo:FlameIonizationDetectorTest</t>
+  </si>
+  <si>
+    <t>Aggregate Soundness Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The percentage of mass lost by degradation as determined by sieving and weighing the samples after the test cycles. </t>
+  </si>
+  <si>
+    <t>aggregate_soundness_value</t>
   </si>
 </sst>
 </file>
@@ -2547,7 +2556,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2585,6 +2594,12 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2600,31 +2615,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2694,6 +2684,31 @@
         <vertAlign val="baseline"/>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2786,8 +2801,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H159" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:H159" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Definitions" displayName="Definitions" ref="A1:H160" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A1:H160" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H159">
     <sortCondition ref="C1:C159"/>
   </sortState>
@@ -2797,29 +2812,29 @@
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="DataType" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="QuantityClass" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Authority" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reference" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D240" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D240" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:D240" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D240">
     <sortCondition ref="B1:B240"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
       <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="SourceElement" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="ConditionalElement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3171,10 +3186,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H159"/>
+  <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6566,6 +6581,27 @@
       </c>
       <c r="F159" s="13" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A160" s="19" t="str">
+        <f>IF(ISNA(VLOOKUP(B160,AssociatedElements!B$2:B3199,1,FALSE)),"Not used","")</f>
+        <v>Not used</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D160" s="20" t="s">
+        <v>781</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F160" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -6600,7 +6636,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+    <sheetView zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>

</xml_diff>

<commit_message>
Updates to triaxial test, properties and draft piling dictionaries
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62878DD1-CEFF-1445-920F-EA96DD1CD152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC50212-9F94-934B-91D8-410102E7ADA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="860" windowWidth="46240" windowHeight="29160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8420" yWindow="860" windowWidth="46240" windowHeight="29160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1746" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="783">
   <si>
     <t>Description</t>
   </si>
@@ -2556,7 +2556,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2598,6 +2598,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2808,7 +2812,7 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="12">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3041,1,FALSE)),"Not used","")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3040,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
@@ -3188,8 +3192,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView topLeftCell="A151" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B160" sqref="B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3233,7 +3237,7 @@
     </row>
     <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3041,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3040,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B2" s="12" t="s">
@@ -3254,7 +3258,7 @@
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B3042,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B3041,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B3" s="2" t="s">
@@ -3275,7 +3279,7 @@
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B3043,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B3042,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" s="2" t="s">
@@ -3296,7 +3300,7 @@
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B3044,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B3043,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B5" s="2" t="s">
@@ -3317,7 +3321,7 @@
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B3045,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B3044,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B6" s="2" t="s">
@@ -3338,7 +3342,7 @@
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B3046,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B3045,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B7" s="13" t="s">
@@ -3359,7 +3363,7 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B3047,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B3046,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B8" s="13" t="s">
@@ -3380,7 +3384,7 @@
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B3048,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B3047,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B9" s="13" t="s">
@@ -3401,7 +3405,7 @@
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B3049,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B3048,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B10" s="13" t="s">
@@ -3424,7 +3428,7 @@
     </row>
     <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B3050,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B3049,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B11" s="13" t="s">
@@ -3447,7 +3451,7 @@
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B3051,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B3050,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B12" s="13" t="s">
@@ -3470,7 +3474,7 @@
     </row>
     <row r="13" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B3169,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B3168,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B13" s="13" t="s">
@@ -3491,7 +3495,7 @@
     </row>
     <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B3052,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B3051,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B14" s="13" t="s">
@@ -3514,7 +3518,7 @@
     </row>
     <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B3053,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B3052,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B15" s="13" t="s">
@@ -3537,7 +3541,7 @@
     </row>
     <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B3170,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B3169,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B16" s="13" t="s">
@@ -3558,7 +3562,7 @@
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B3055,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B3054,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B17" s="13" t="s">
@@ -3581,7 +3585,7 @@
     </row>
     <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B3191,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B3190,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B18" s="13" t="s">
@@ -3602,7 +3606,7 @@
     </row>
     <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B3192,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B3191,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B19" s="13" t="s">
@@ -3623,7 +3627,7 @@
     </row>
     <row r="20" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B3058,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B3057,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B20" s="13" t="s">
@@ -3646,7 +3650,7 @@
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B3059,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B3058,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B21" s="13" t="s">
@@ -3669,7 +3673,7 @@
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B3060,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B3059,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B22" s="13" t="s">
@@ -3692,7 +3696,7 @@
     </row>
     <row r="23" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B3061,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B3060,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B23" s="13" t="s">
@@ -3715,7 +3719,7 @@
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B3064,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B3063,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B24" s="13" t="s">
@@ -3738,7 +3742,7 @@
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B3065,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B3064,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B25" s="13" t="s">
@@ -3761,7 +3765,7 @@
     </row>
     <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B3062,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B3061,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B26" s="13" t="s">
@@ -3784,7 +3788,7 @@
     </row>
     <row r="27" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B3066,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B3065,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B27" s="13" t="s">
@@ -3807,7 +3811,7 @@
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B3067,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B3066,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B28" s="13" t="s">
@@ -3830,7 +3834,7 @@
     </row>
     <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B3070,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B3069,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B29" s="13" t="s">
@@ -3851,7 +3855,7 @@
     </row>
     <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B3063,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B3062,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B30" s="13" t="s">
@@ -3874,7 +3878,7 @@
     </row>
     <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B3073,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B3072,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B31" s="13" t="s">
@@ -3895,7 +3899,7 @@
     </row>
     <row r="32" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B3074,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B3073,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B32" s="13" t="s">
@@ -3916,7 +3920,7 @@
     </row>
     <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B3076,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B3075,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B33" s="13" t="s">
@@ -3937,7 +3941,7 @@
     </row>
     <row r="34" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B3077,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B3076,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B34" s="13" t="s">
@@ -3958,7 +3962,7 @@
     </row>
     <row r="35" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B3078,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B3077,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B35" s="13" t="s">
@@ -3979,7 +3983,7 @@
     </row>
     <row r="36" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B3056,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B3055,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B36" s="13" t="s">
@@ -4002,7 +4006,7 @@
     </row>
     <row r="37" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B3057,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B3056,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B37" s="13" t="s">
@@ -4025,7 +4029,7 @@
     </row>
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B3181,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B3180,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B38" s="13" t="s">
@@ -4046,7 +4050,7 @@
     </row>
     <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B3093,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B3092,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B39" s="13" t="s">
@@ -4067,7 +4071,7 @@
     </row>
     <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B3079,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B3078,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B40" s="13" t="s">
@@ -4088,7 +4092,7 @@
     </row>
     <row r="41" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B3080,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B3079,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B41" s="13" t="s">
@@ -4109,7 +4113,7 @@
     </row>
     <row r="42" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B3081,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B3080,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B42" s="13" t="s">
@@ -4130,7 +4134,7 @@
     </row>
     <row r="43" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B3082,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B3081,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B43" s="13" t="s">
@@ -4151,7 +4155,7 @@
     </row>
     <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B3083,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B3082,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B44" s="13" t="s">
@@ -4172,7 +4176,7 @@
     </row>
     <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B45,AssociatedElements!B$2:B3054,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B45,AssociatedElements!B$2:B3053,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B45" s="13" t="s">
@@ -4195,7 +4199,7 @@
     </row>
     <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B46,AssociatedElements!B$2:B3087,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B46,AssociatedElements!B$2:B3086,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B46" s="13" t="s">
@@ -4216,7 +4220,7 @@
     </row>
     <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B47,AssociatedElements!B$2:B3150,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B47,AssociatedElements!B$2:B3149,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B47" s="13" t="s">
@@ -4237,7 +4241,7 @@
     </row>
     <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B48,AssociatedElements!B$2:B3084,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B48,AssociatedElements!B$2:B3083,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B48" s="13" t="s">
@@ -4258,7 +4262,7 @@
     </row>
     <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B49,AssociatedElements!B$2:B3085,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B49,AssociatedElements!B$2:B3084,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B49" s="13" t="s">
@@ -4279,7 +4283,7 @@
     </row>
     <row r="50" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B50,AssociatedElements!B$2:B3086,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B50,AssociatedElements!B$2:B3085,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B50" s="13" t="s">
@@ -4300,7 +4304,7 @@
     </row>
     <row r="51" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B51,AssociatedElements!B$2:B3141,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B51,AssociatedElements!B$2:B3140,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B51" s="13" t="s">
@@ -4321,7 +4325,7 @@
     </row>
     <row r="52" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B52,AssociatedElements!B$2:B3142,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B52,AssociatedElements!B$2:B3141,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B52" s="13" t="s">
@@ -4342,7 +4346,7 @@
     </row>
     <row r="53" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B53,AssociatedElements!B$2:B3193,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B53,AssociatedElements!B$2:B3192,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B53" s="13" t="s">
@@ -4363,7 +4367,7 @@
     </row>
     <row r="54" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B54,AssociatedElements!B$2:B3194,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B54,AssociatedElements!B$2:B3193,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B54" s="13" t="s">
@@ -4384,7 +4388,7 @@
     </row>
     <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B55,AssociatedElements!B$2:B3090,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B55,AssociatedElements!B$2:B3089,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B55" s="13" t="s">
@@ -4405,7 +4409,7 @@
     </row>
     <row r="56" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B56,AssociatedElements!B$2:B3091,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B56,AssociatedElements!B$2:B3090,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B56" s="13" t="s">
@@ -4426,7 +4430,7 @@
     </row>
     <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B57,AssociatedElements!B$2:B3092,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B57,AssociatedElements!B$2:B3091,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B57" s="13" t="s">
@@ -4447,7 +4451,7 @@
     </row>
     <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B58,AssociatedElements!B$2:B3096,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B58,AssociatedElements!B$2:B3095,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B58" s="13" t="s">
@@ -4468,7 +4472,7 @@
     </row>
     <row r="59" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B59,AssociatedElements!B$2:B3097,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B59,AssociatedElements!B$2:B3096,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B59" s="13" t="s">
@@ -4489,7 +4493,7 @@
     </row>
     <row r="60" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B60,AssociatedElements!B$2:B3098,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B60,AssociatedElements!B$2:B3097,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B60" s="13" t="s">
@@ -4510,7 +4514,7 @@
     </row>
     <row r="61" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B61,AssociatedElements!B$2:B3099,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B61,AssociatedElements!B$2:B3098,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B61" s="13" t="s">
@@ -4531,7 +4535,7 @@
     </row>
     <row r="62" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B62,AssociatedElements!B$2:B3068,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B62,AssociatedElements!B$2:B3067,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B62" s="13" t="s">
@@ -4554,7 +4558,7 @@
     </row>
     <row r="63" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B63,AssociatedElements!B$2:B3100,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B63,AssociatedElements!B$2:B3099,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B63" s="13" t="s">
@@ -4575,7 +4579,7 @@
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B64,AssociatedElements!B$2:B3101,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B64,AssociatedElements!B$2:B3100,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B64" s="13" t="s">
@@ -4596,7 +4600,7 @@
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B65,AssociatedElements!B$2:B3104,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B65,AssociatedElements!B$2:B3103,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B65" s="13" t="s">
@@ -4617,7 +4621,7 @@
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B66,AssociatedElements!B$2:B3107,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B66,AssociatedElements!B$2:B3106,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B66" s="13" t="s">
@@ -4638,7 +4642,7 @@
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B67,AssociatedElements!B$2:B3108,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B67,AssociatedElements!B$2:B3107,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B67" s="13" t="s">
@@ -4659,7 +4663,7 @@
     </row>
     <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B68,AssociatedElements!B$2:B3109,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B68,AssociatedElements!B$2:B3108,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B68" s="13" t="s">
@@ -4680,7 +4684,7 @@
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B69,AssociatedElements!B$2:B3110,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B69,AssociatedElements!B$2:B3109,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B69" s="13" t="s">
@@ -4701,7 +4705,7 @@
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B70,AssociatedElements!B$2:B3111,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B70,AssociatedElements!B$2:B3110,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B70" s="13" t="s">
@@ -4722,7 +4726,7 @@
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B71,AssociatedElements!B$2:B3112,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B71,AssociatedElements!B$2:B3111,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B71" s="13" t="s">
@@ -4743,7 +4747,7 @@
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B72,AssociatedElements!B$2:B3113,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B72,AssociatedElements!B$2:B3112,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B72" s="13" t="s">
@@ -4764,7 +4768,7 @@
     </row>
     <row r="73" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B73,AssociatedElements!B$2:B3115,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B73,AssociatedElements!B$2:B3114,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B73" s="13" t="s">
@@ -4785,7 +4789,7 @@
     </row>
     <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B74,AssociatedElements!B$2:B3117,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B74,AssociatedElements!B$2:B3116,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B74" s="13" t="s">
@@ -4806,7 +4810,7 @@
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B75,AssociatedElements!B$2:B3118,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B75,AssociatedElements!B$2:B3117,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B75" s="13" t="s">
@@ -4827,7 +4831,7 @@
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B76,AssociatedElements!B$2:B3119,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B76,AssociatedElements!B$2:B3118,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B76" s="13" t="s">
@@ -4848,7 +4852,7 @@
     </row>
     <row r="77" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B77,AssociatedElements!B$2:B3088,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B77,AssociatedElements!B$2:B3087,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B77" s="13" t="s">
@@ -4869,7 +4873,7 @@
     </row>
     <row r="78" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B78,AssociatedElements!B$2:B3120,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B78,AssociatedElements!B$2:B3119,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B78" s="13" t="s">
@@ -4890,7 +4894,7 @@
     </row>
     <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B79,AssociatedElements!B$2:B3123,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B79,AssociatedElements!B$2:B3122,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B79" s="13" t="s">
@@ -4911,7 +4915,7 @@
     </row>
     <row r="80" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B80,AssociatedElements!B$2:B3124,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B80,AssociatedElements!B$2:B3123,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B80" s="13" t="s">
@@ -4932,7 +4936,7 @@
     </row>
     <row r="81" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B81,AssociatedElements!B$2:B3125,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B81,AssociatedElements!B$2:B3124,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B81" s="13" t="s">
@@ -4953,7 +4957,7 @@
     </row>
     <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B82,AssociatedElements!B$2:B3126,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B82,AssociatedElements!B$2:B3125,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B82" s="13" t="s">
@@ -4974,7 +4978,7 @@
     </row>
     <row r="83" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B83,AssociatedElements!B$2:B3189,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B83,AssociatedElements!B$2:B3188,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B83" s="13" t="s">
@@ -4995,7 +4999,7 @@
     </row>
     <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B84,AssociatedElements!B$2:B3127,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B84,AssociatedElements!B$2:B3126,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B84" s="13" t="s">
@@ -5016,7 +5020,7 @@
     </row>
     <row r="85" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B85,AssociatedElements!B$2:B3190,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B85,AssociatedElements!B$2:B3189,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B85" s="13" t="s">
@@ -5037,7 +5041,7 @@
     </row>
     <row r="86" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B86,AssociatedElements!B$2:B3116,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B86,AssociatedElements!B$2:B3115,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B86" s="13" t="s">
@@ -5058,7 +5062,7 @@
     </row>
     <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B87,AssociatedElements!B$2:B3114,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B87,AssociatedElements!B$2:B3113,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B87" s="13" t="s">
@@ -5079,7 +5083,7 @@
     </row>
     <row r="88" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B88,AssociatedElements!B$2:B3128,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B88,AssociatedElements!B$2:B3127,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B88" s="13" t="s">
@@ -5100,7 +5104,7 @@
     </row>
     <row r="89" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B89,AssociatedElements!B$2:B3129,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B89,AssociatedElements!B$2:B3128,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B89" s="13" t="s">
@@ -5121,7 +5125,7 @@
     </row>
     <row r="90" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B90,AssociatedElements!B$2:B3130,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B90,AssociatedElements!B$2:B3129,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B90" s="13" t="s">
@@ -5142,7 +5146,7 @@
     </row>
     <row r="91" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B91,AssociatedElements!B$2:B3131,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B91,AssociatedElements!B$2:B3130,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B91" s="13" t="s">
@@ -5163,7 +5167,7 @@
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B92,AssociatedElements!B$2:B3094,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B92,AssociatedElements!B$2:B3093,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B92" s="13" t="s">
@@ -5184,7 +5188,7 @@
     </row>
     <row r="93" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B93,AssociatedElements!B$2:B3071,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B93,AssociatedElements!B$2:B3070,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B93" s="13" t="s">
@@ -5205,7 +5209,7 @@
     </row>
     <row r="94" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B94,AssociatedElements!B$2:B3156,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B94,AssociatedElements!B$2:B3155,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B94" s="13" t="s">
@@ -5226,7 +5230,7 @@
     </row>
     <row r="95" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B95,AssociatedElements!B$2:B3157,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B95,AssociatedElements!B$2:B3156,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B95" s="13" t="s">
@@ -5247,7 +5251,7 @@
     </row>
     <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B96,AssociatedElements!B$2:B3132,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B96,AssociatedElements!B$2:B3131,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B96" s="13" t="s">
@@ -5268,7 +5272,7 @@
     </row>
     <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B97,AssociatedElements!B$2:B3133,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B97,AssociatedElements!B$2:B3132,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B97" s="13" t="s">
@@ -5289,7 +5293,7 @@
     </row>
     <row r="98" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B98,AssociatedElements!B$2:B3134,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B98,AssociatedElements!B$2:B3133,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B98" s="13" t="s">
@@ -5310,7 +5314,7 @@
     </row>
     <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B99,AssociatedElements!B$2:B3135,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B99,AssociatedElements!B$2:B3134,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B99" s="13" t="s">
@@ -5331,7 +5335,7 @@
     </row>
     <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B100,AssociatedElements!B$2:B3136,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B100,AssociatedElements!B$2:B3135,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B100" s="13" t="s">
@@ -5352,7 +5356,7 @@
     </row>
     <row r="101" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B101,AssociatedElements!B$2:B3137,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B101,AssociatedElements!B$2:B3136,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B101" s="13" t="s">
@@ -5373,7 +5377,7 @@
     </row>
     <row r="102" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B102,AssociatedElements!B$2:B3138,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B102,AssociatedElements!B$2:B3137,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B102" s="13" t="s">
@@ -5394,7 +5398,7 @@
     </row>
     <row r="103" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B103,AssociatedElements!B$2:B3139,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B103,AssociatedElements!B$2:B3138,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B103" s="13" t="s">
@@ -5415,7 +5419,7 @@
     </row>
     <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B104,AssociatedElements!B$2:B3140,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B104,AssociatedElements!B$2:B3139,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B104" s="13" t="s">
@@ -5436,7 +5440,7 @@
     </row>
     <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B105,AssociatedElements!B$2:B3143,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B105,AssociatedElements!B$2:B3142,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B105" s="13" t="s">
@@ -5457,7 +5461,7 @@
     </row>
     <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B106,AssociatedElements!B$2:B3144,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B106,AssociatedElements!B$2:B3143,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B106" s="13" t="s">
@@ -5478,7 +5482,7 @@
     </row>
     <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B107,AssociatedElements!B$2:B3145,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B107,AssociatedElements!B$2:B3144,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B107" s="13" t="s">
@@ -5499,7 +5503,7 @@
     </row>
     <row r="108" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B108,AssociatedElements!B$2:B3146,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B108,AssociatedElements!B$2:B3145,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B108" s="13" t="s">
@@ -5520,7 +5524,7 @@
     </row>
     <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B109,AssociatedElements!B$2:B3147,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B109,AssociatedElements!B$2:B3146,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B109" s="13" t="s">
@@ -5541,7 +5545,7 @@
     </row>
     <row r="110" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B110,AssociatedElements!B$2:B3198,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B110,AssociatedElements!B$2:B3197,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B110" s="2" t="s">
@@ -5562,7 +5566,7 @@
     </row>
     <row r="111" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B111,AssociatedElements!B$2:B3148,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B111,AssociatedElements!B$2:B3147,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B111" s="13" t="s">
@@ -5583,7 +5587,7 @@
     </row>
     <row r="112" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B112,AssociatedElements!B$2:B3149,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B112,AssociatedElements!B$2:B3148,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B112" s="13" t="s">
@@ -5604,7 +5608,7 @@
     </row>
     <row r="113" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B113,AssociatedElements!B$2:B3095,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B113,AssociatedElements!B$2:B3094,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B113" s="13" t="s">
@@ -5625,7 +5629,7 @@
     </row>
     <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B114,AssociatedElements!B$2:B3072,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B114,AssociatedElements!B$2:B3071,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B114" s="13" t="s">
@@ -5646,7 +5650,7 @@
     </row>
     <row r="115" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B115,AssociatedElements!B$2:B3158,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B115,AssociatedElements!B$2:B3157,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B115" s="13" t="s">
@@ -5667,7 +5671,7 @@
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B116,AssociatedElements!B$2:B3151,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B116,AssociatedElements!B$2:B3150,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B116" s="13" t="s">
@@ -5688,7 +5692,7 @@
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B117,AssociatedElements!B$2:B3152,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B117,AssociatedElements!B$2:B3151,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B117" s="13" t="s">
@@ -5709,7 +5713,7 @@
     </row>
     <row r="118" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B118,AssociatedElements!B$2:B3153,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B118,AssociatedElements!B$2:B3152,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B118" s="13" t="s">
@@ -5730,7 +5734,7 @@
     </row>
     <row r="119" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B119,AssociatedElements!B$2:B3154,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B119,AssociatedElements!B$2:B3153,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B119" s="13" t="s">
@@ -5751,7 +5755,7 @@
     </row>
     <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B120,AssociatedElements!B$2:B3155,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B120,AssociatedElements!B$2:B3154,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B120" s="13" t="s">
@@ -5772,7 +5776,7 @@
     </row>
     <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B121,AssociatedElements!B$2:B3121,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B121,AssociatedElements!B$2:B3120,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B121" s="13" t="s">
@@ -5793,7 +5797,7 @@
     </row>
     <row r="122" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B122,AssociatedElements!B$2:B3197,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B122,AssociatedElements!B$2:B3196,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B122" s="2" t="s">
@@ -5814,7 +5818,7 @@
     </row>
     <row r="123" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B123,AssociatedElements!B$2:B3159,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B123,AssociatedElements!B$2:B3158,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B123" s="13" t="s">
@@ -5835,7 +5839,7 @@
     </row>
     <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B124,AssociatedElements!B$2:B3160,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B124,AssociatedElements!B$2:B3159,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B124" s="13" t="s">
@@ -5856,7 +5860,7 @@
     </row>
     <row r="125" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B125,AssociatedElements!B$2:B3161,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B125,AssociatedElements!B$2:B3160,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B125" s="13" t="s">
@@ -5877,7 +5881,7 @@
     </row>
     <row r="126" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B126,AssociatedElements!B$2:B3162,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B126,AssociatedElements!B$2:B3161,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B126" s="13" t="s">
@@ -5898,7 +5902,7 @@
     </row>
     <row r="127" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B127,AssociatedElements!B$2:B3106,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B127,AssociatedElements!B$2:B3105,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B127" s="13" t="s">
@@ -5919,7 +5923,7 @@
     </row>
     <row r="128" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B128,AssociatedElements!B$2:B3163,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B128,AssociatedElements!B$2:B3162,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B128" s="13" t="s">
@@ -5940,7 +5944,7 @@
     </row>
     <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B129,AssociatedElements!B$2:B3164,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B129,AssociatedElements!B$2:B3163,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B129" s="13" t="s">
@@ -5961,7 +5965,7 @@
     </row>
     <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B130,AssociatedElements!B$2:B3165,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B130,AssociatedElements!B$2:B3164,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B130" s="13" t="s">
@@ -5982,7 +5986,7 @@
     </row>
     <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B131,AssociatedElements!B$2:B3166,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B131,AssociatedElements!B$2:B3165,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B131" s="13" t="s">
@@ -6003,7 +6007,7 @@
     </row>
     <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B132,AssociatedElements!B$2:B3167,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B132,AssociatedElements!B$2:B3166,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B132" s="13" t="s">
@@ -6024,7 +6028,7 @@
     </row>
     <row r="133" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B133,AssociatedElements!B$2:B3168,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B133,AssociatedElements!B$2:B3167,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B133" s="13" t="s">
@@ -6043,7 +6047,7 @@
     </row>
     <row r="134" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B134,AssociatedElements!B$2:B3171,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B134,AssociatedElements!B$2:B3170,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B134" s="13" t="s">
@@ -6064,7 +6068,7 @@
     </row>
     <row r="135" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B135,AssociatedElements!B$2:B3172,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B135,AssociatedElements!B$2:B3171,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B135" s="13" t="s">
@@ -6085,7 +6089,7 @@
     </row>
     <row r="136" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B136,AssociatedElements!B$2:B3174,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B136,AssociatedElements!B$2:B3173,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B136" s="13" t="s">
@@ -6106,7 +6110,7 @@
     </row>
     <row r="137" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B137,AssociatedElements!B$2:B3173,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B137,AssociatedElements!B$2:B3172,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B137" s="13" t="s">
@@ -6127,7 +6131,7 @@
     </row>
     <row r="138" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B138,AssociatedElements!B$2:B3175,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B138,AssociatedElements!B$2:B3174,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B138" s="13" t="s">
@@ -6148,7 +6152,7 @@
     </row>
     <row r="139" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B139,AssociatedElements!B$2:B3176,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B139,AssociatedElements!B$2:B3175,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B139" s="13" t="s">
@@ -6169,7 +6173,7 @@
     </row>
     <row r="140" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B140,AssociatedElements!B$2:B3177,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B140,AssociatedElements!B$2:B3176,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B140" s="13" t="s">
@@ -6190,7 +6194,7 @@
     </row>
     <row r="141" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B141,AssociatedElements!B$2:B3178,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B141,AssociatedElements!B$2:B3177,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B141" s="13" t="s">
@@ -6211,7 +6215,7 @@
     </row>
     <row r="142" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B142,AssociatedElements!B$2:B3179,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B142,AssociatedElements!B$2:B3178,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B142" s="13" t="s">
@@ -6232,7 +6236,7 @@
     </row>
     <row r="143" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B143,AssociatedElements!B$2:B3180,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B143,AssociatedElements!B$2:B3179,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B143" s="13" t="s">
@@ -6253,7 +6257,7 @@
     </row>
     <row r="144" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B144,AssociatedElements!B$2:B3186,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B144,AssociatedElements!B$2:B3185,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B144" s="13" t="s">
@@ -6274,7 +6278,7 @@
     </row>
     <row r="145" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B145,AssociatedElements!B$2:B3182,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B145,AssociatedElements!B$2:B3181,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B145" s="13" t="s">
@@ -6295,7 +6299,7 @@
     </row>
     <row r="146" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B146,AssociatedElements!B$2:B3075,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B146,AssociatedElements!B$2:B3074,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B146" s="13" t="s">
@@ -6316,7 +6320,7 @@
     </row>
     <row r="147" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B147,AssociatedElements!B$2:B3105,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B147,AssociatedElements!B$2:B3104,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B147" s="13" t="s">
@@ -6337,7 +6341,7 @@
     </row>
     <row r="148" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B148,AssociatedElements!B$2:B3183,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B148,AssociatedElements!B$2:B3182,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B148" s="13" t="s">
@@ -6358,7 +6362,7 @@
     </row>
     <row r="149" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B149,AssociatedElements!B$2:B3184,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B149,AssociatedElements!B$2:B3183,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B149" s="13" t="s">
@@ -6377,7 +6381,7 @@
     </row>
     <row r="150" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B150,AssociatedElements!B$2:B3185,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B150,AssociatedElements!B$2:B3184,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B150" s="13" t="s">
@@ -6396,7 +6400,7 @@
     </row>
     <row r="151" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B151,AssociatedElements!B$2:B3069,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B151,AssociatedElements!B$2:B3068,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B151" s="13" t="s">
@@ -6419,7 +6423,7 @@
     </row>
     <row r="152" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B152,AssociatedElements!B$2:B3089,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B152,AssociatedElements!B$2:B3088,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B152" s="13" t="s">
@@ -6440,7 +6444,7 @@
     </row>
     <row r="153" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B153,AssociatedElements!B$2:B3187,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B153,AssociatedElements!B$2:B3186,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B153" s="13" t="s">
@@ -6461,7 +6465,7 @@
     </row>
     <row r="154" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B154,AssociatedElements!B$2:B3188,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B154,AssociatedElements!B$2:B3187,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B154" s="13" t="s">
@@ -6480,7 +6484,7 @@
     </row>
     <row r="155" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B155,AssociatedElements!B$2:B3191,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B155,AssociatedElements!B$2:B3190,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B155" s="13" t="s">
@@ -6501,7 +6505,7 @@
     </row>
     <row r="156" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B156,AssociatedElements!B$2:B3191,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B156,AssociatedElements!B$2:B3190,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B156" s="13" t="s">
@@ -6522,7 +6526,7 @@
     </row>
     <row r="157" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B157,AssociatedElements!B$2:B3102,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B157,AssociatedElements!B$2:B3101,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B157" s="13" t="s">
@@ -6543,7 +6547,7 @@
     </row>
     <row r="158" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B158,AssociatedElements!B$2:B3103,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B158,AssociatedElements!B$2:B3102,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B158" s="13" t="s">
@@ -6564,7 +6568,7 @@
     </row>
     <row r="159" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B159,AssociatedElements!B$2:B3122,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B159,AssociatedElements!B$2:B3121,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B159" s="13" t="s">
@@ -6585,8 +6589,8 @@
     </row>
     <row r="160" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" s="19" t="str">
-        <f>IF(ISNA(VLOOKUP(B160,AssociatedElements!B$2:B3199,1,FALSE)),"Not used","")</f>
-        <v>Not used</v>
+        <f>IF(ISNA(VLOOKUP(B160,AssociatedElements!B$2:B3198,1,FALSE)),"Not used","")</f>
+        <v/>
       </c>
       <c r="B160" s="2" t="s">
         <v>782</v>
@@ -6636,9 +6640,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D240"/>
   <sheetViews>
-    <sheetView zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D236" sqref="D236:D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6813,19 +6817,19 @@
         <v>746</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="21" t="str">
         <f>IF(ISNA(VLOOKUP(B12,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B12" t="s">
-        <v>243</v>
+      <c r="B12" s="22" t="s">
+        <v>782</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D12" t="s">
-        <v>750</v>
+      <c r="D12" s="4" t="s">
+        <v>748</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -6834,13 +6838,13 @@
         <v/>
       </c>
       <c r="B13" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>279</v>
+      <c r="D13" t="s">
+        <v>750</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -6849,13 +6853,13 @@
         <v/>
       </c>
       <c r="B14" t="s">
-        <v>398</v>
+        <v>280</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>399</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -6864,13 +6868,13 @@
         <v/>
       </c>
       <c r="B15" t="s">
-        <v>301</v>
+        <v>398</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>302</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -6885,7 +6889,7 @@
         <v>724</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -6900,7 +6904,7 @@
         <v>724</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -6914,8 +6918,8 @@
       <c r="C18" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D18" t="s">
-        <v>754</v>
+      <c r="D18" s="4" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -6924,13 +6928,13 @@
         <v/>
       </c>
       <c r="B19" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>279</v>
+      <c r="D19" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -6939,13 +6943,13 @@
         <v/>
       </c>
       <c r="B20" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>302</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -6960,7 +6964,7 @@
         <v>724</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -6969,13 +6973,13 @@
         <v/>
       </c>
       <c r="B22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -6990,7 +6994,7 @@
         <v>724</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -6999,13 +7003,13 @@
         <v/>
       </c>
       <c r="B24" t="s">
-        <v>256</v>
+        <v>304</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D24" t="s">
-        <v>752</v>
+      <c r="D24" s="4" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -7014,13 +7018,13 @@
         <v/>
       </c>
       <c r="B25" t="s">
-        <v>312</v>
+        <v>256</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>313</v>
+      <c r="D25" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -7029,13 +7033,13 @@
         <v/>
       </c>
       <c r="B26" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -7044,7 +7048,7 @@
         <v/>
       </c>
       <c r="B27" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>724</v>
@@ -7059,13 +7063,13 @@
         <v/>
       </c>
       <c r="B28" t="s">
-        <v>282</v>
+        <v>336</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>279</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -7080,7 +7084,7 @@
         <v>724</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>355</v>
+        <v>279</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -7089,43 +7093,43 @@
         <v/>
       </c>
       <c r="B30" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="str">
+        <f>IF(ISNA(VLOOKUP(B31,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B31" t="s">
         <v>257</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="str">
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" t="str">
         <f>IF(ISNA(VLOOKUP(#REF!,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C32" s="4" t="s">
+        <v>724</v>
+      </c>
+      <c r="D32" t="s">
         <v>763</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B32" t="s">
-        <v>337</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>724</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -7134,13 +7138,13 @@
         <v/>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>337</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>279</v>
+        <v>335</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -7154,8 +7158,8 @@
       <c r="C34" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D34" t="s">
-        <v>764</v>
+      <c r="D34" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -7164,13 +7168,13 @@
         <v/>
       </c>
       <c r="B35" t="s">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>323</v>
+      <c r="D35" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -7185,7 +7189,7 @@
         <v>724</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -7199,8 +7203,8 @@
       <c r="C37" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D37" t="s">
-        <v>755</v>
+      <c r="D37" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -7215,7 +7219,7 @@
         <v>724</v>
       </c>
       <c r="D38" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -7224,13 +7228,13 @@
         <v/>
       </c>
       <c r="B39" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>323</v>
+      <c r="D39" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -7239,7 +7243,7 @@
         <v/>
       </c>
       <c r="B40" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>724</v>
@@ -7260,7 +7264,7 @@
         <v>724</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>355</v>
+        <v>323</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -7275,7 +7279,7 @@
         <v>724</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -7289,8 +7293,8 @@
       <c r="C43" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D43" t="s">
-        <v>755</v>
+      <c r="D43" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -7305,7 +7309,7 @@
         <v>724</v>
       </c>
       <c r="D44" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -7314,13 +7318,13 @@
         <v/>
       </c>
       <c r="B45" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>323</v>
+      <c r="D45" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -7335,7 +7339,7 @@
         <v>724</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -7349,8 +7353,8 @@
       <c r="C47" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D47" t="s">
-        <v>755</v>
+      <c r="D47" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -7365,37 +7369,37 @@
         <v>724</v>
       </c>
       <c r="D48" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f>IF(ISNA(VLOOKUP(B49,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>338</v>
+      <c r="B49" t="s">
+        <v>308</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D49" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f>IF(ISNA(VLOOKUP(B50,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>338</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D50" s="4" t="s">
-        <v>335</v>
+      <c r="D50" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -7404,13 +7408,13 @@
         <v/>
       </c>
       <c r="B51" t="s">
-        <v>264</v>
+        <v>338</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>265</v>
+        <v>335</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -7419,7 +7423,7 @@
         <v/>
       </c>
       <c r="B52" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>724</v>
@@ -7434,13 +7438,13 @@
         <v/>
       </c>
       <c r="B53" t="s">
-        <v>339</v>
+        <v>266</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>335</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -7449,13 +7453,13 @@
         <v/>
       </c>
       <c r="B54" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>258</v>
+        <v>335</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -7464,13 +7468,13 @@
         <v/>
       </c>
       <c r="B55" t="s">
-        <v>321</v>
+        <v>259</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>350</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -7485,7 +7489,7 @@
         <v>724</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>393</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -7499,8 +7503,8 @@
       <c r="C57" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D57" t="s">
-        <v>770</v>
+      <c r="D57" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -7509,13 +7513,13 @@
         <v/>
       </c>
       <c r="B58" t="s">
-        <v>374</v>
+        <v>321</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>373</v>
+      <c r="D58" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -7524,13 +7528,13 @@
         <v/>
       </c>
       <c r="B59" t="s">
-        <v>244</v>
+        <v>374</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>245</v>
+        <v>373</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -7545,7 +7549,7 @@
         <v>724</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>396</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -7554,13 +7558,13 @@
         <v/>
       </c>
       <c r="B61" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>258</v>
+        <v>396</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -7575,127 +7579,127 @@
         <v>724</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f>IF(ISNA(VLOOKUP(B63,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>340</v>
+      <c r="B63" t="s">
+        <v>260</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D63" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D63" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f>IF(ISNA(VLOOKUP(B64,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>340</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D64" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f>IF(ISNA(VLOOKUP(B65,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>341</v>
+      <c r="B65" t="s">
+        <v>340</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D65" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f>IF(ISNA(VLOOKUP(B66,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>341</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D66" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f>IF(ISNA(VLOOKUP(B67,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>342</v>
+      <c r="B67" t="s">
+        <v>341</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D67" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f>IF(ISNA(VLOOKUP(B68,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D68" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f>IF(ISNA(VLOOKUP(B69,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>343</v>
+      <c r="B69" t="s">
+        <v>342</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D69" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
         <f>IF(ISNA(VLOOKUP(B70,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>343</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D70" s="4" t="s">
-        <v>335</v>
+      <c r="D70" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -7704,13 +7708,13 @@
         <v/>
       </c>
       <c r="B71" t="s">
-        <v>397</v>
+        <v>343</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>396</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -7719,13 +7723,13 @@
         <v/>
       </c>
       <c r="B72" t="s">
-        <v>360</v>
+        <v>397</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D72" t="s">
-        <v>764</v>
+      <c r="D72" s="4" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -7734,13 +7738,13 @@
         <v/>
       </c>
       <c r="B73" t="s">
-        <v>284</v>
+        <v>360</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>279</v>
+      <c r="D73" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -7749,7 +7753,7 @@
         <v/>
       </c>
       <c r="B74" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>724</v>
@@ -7764,13 +7768,13 @@
         <v/>
       </c>
       <c r="B75" t="s">
-        <v>320</v>
+        <v>285</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -7779,13 +7783,13 @@
         <v/>
       </c>
       <c r="B76" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -7794,13 +7798,13 @@
         <v/>
       </c>
       <c r="B77" t="s">
-        <v>286</v>
+        <v>316</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -7809,13 +7813,13 @@
         <v/>
       </c>
       <c r="B78" t="s">
-        <v>413</v>
+        <v>286</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>414</v>
+        <v>279</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -7824,13 +7828,13 @@
         <v/>
       </c>
       <c r="B79" t="s">
-        <v>277</v>
+        <v>413</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D79" t="s">
-        <v>276</v>
+      <c r="D79" s="4" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -7844,8 +7848,8 @@
       <c r="C80" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D80" s="4" t="s">
-        <v>779</v>
+      <c r="D80" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -7854,13 +7858,13 @@
         <v/>
       </c>
       <c r="B81" t="s">
-        <v>400</v>
+        <v>277</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>401</v>
+        <v>779</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -7869,13 +7873,13 @@
         <v/>
       </c>
       <c r="B82" t="s">
-        <v>267</v>
+        <v>400</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>265</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -7889,8 +7893,8 @@
       <c r="C83" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D83" t="s">
-        <v>764</v>
+      <c r="D83" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -7899,13 +7903,13 @@
         <v/>
       </c>
       <c r="B84" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>265</v>
+      <c r="D84" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -7920,7 +7924,7 @@
         <v>724</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -7935,7 +7939,7 @@
         <v>724</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>392</v>
+        <v>279</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -7950,7 +7954,7 @@
         <v>724</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>772</v>
+        <v>392</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -7959,13 +7963,13 @@
         <v/>
       </c>
       <c r="B88" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>265</v>
+        <v>772</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -7980,7 +7984,7 @@
         <v>724</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -7995,7 +7999,7 @@
         <v>724</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>392</v>
+        <v>279</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -8009,8 +8013,8 @@
       <c r="C91" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D91" t="s">
-        <v>764</v>
+      <c r="D91" s="4" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -8024,8 +8028,8 @@
       <c r="C92" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D92" s="4" t="s">
-        <v>772</v>
+      <c r="D92" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -8034,13 +8038,13 @@
         <v/>
       </c>
       <c r="B93" t="s">
-        <v>375</v>
+        <v>269</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>373</v>
+        <v>772</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -8049,13 +8053,13 @@
         <v/>
       </c>
       <c r="B94" t="s">
-        <v>300</v>
+        <v>375</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D94" t="s">
-        <v>753</v>
+      <c r="D94" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -8064,13 +8068,13 @@
         <v/>
       </c>
       <c r="B95" t="s">
-        <v>426</v>
+        <v>300</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D95" t="s">
-        <v>425</v>
+        <v>753</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -8084,8 +8088,8 @@
       <c r="C96" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>427</v>
+      <c r="D96" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -8094,13 +8098,13 @@
         <v/>
       </c>
       <c r="B97" t="s">
-        <v>376</v>
+        <v>426</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>373</v>
+        <v>427</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -8109,13 +8113,13 @@
         <v/>
       </c>
       <c r="B98" t="s">
-        <v>287</v>
+        <v>376</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>279</v>
+        <v>373</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -8124,13 +8128,13 @@
         <v/>
       </c>
       <c r="B99" t="s">
-        <v>377</v>
+        <v>287</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>373</v>
+        <v>279</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -8145,7 +8149,7 @@
         <v>724</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>725</v>
+        <v>373</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -8154,13 +8158,13 @@
         <v/>
       </c>
       <c r="B101" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>373</v>
+        <v>725</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -8175,7 +8179,7 @@
         <v>724</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>725</v>
+        <v>373</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -8184,13 +8188,13 @@
         <v/>
       </c>
       <c r="B103" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>373</v>
+        <v>725</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -8205,7 +8209,7 @@
         <v>724</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>725</v>
+        <v>373</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -8214,13 +8218,13 @@
         <v/>
       </c>
       <c r="B105" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D105" t="s">
-        <v>764</v>
+      <c r="D105" s="4" t="s">
+        <v>725</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -8229,13 +8233,13 @@
         <v/>
       </c>
       <c r="B106" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D106" s="4" t="s">
-        <v>352</v>
+      <c r="D106" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -8244,7 +8248,7 @@
         <v/>
       </c>
       <c r="B107" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>724</v>
@@ -8259,13 +8263,13 @@
         <v/>
       </c>
       <c r="B108" t="s">
-        <v>380</v>
+        <v>353</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -8274,13 +8278,13 @@
         <v/>
       </c>
       <c r="B109" t="s">
-        <v>362</v>
+        <v>380</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D109" t="s">
-        <v>764</v>
+      <c r="D109" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -8289,13 +8293,13 @@
         <v/>
       </c>
       <c r="B110" t="s">
-        <v>402</v>
+        <v>362</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D110" s="4" t="s">
-        <v>403</v>
+      <c r="D110" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -8304,7 +8308,7 @@
         <v/>
       </c>
       <c r="B111" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>724</v>
@@ -8319,7 +8323,7 @@
         <v/>
       </c>
       <c r="B112" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>724</v>
@@ -8334,7 +8338,7 @@
         <v/>
       </c>
       <c r="B113" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>724</v>
@@ -8349,13 +8353,13 @@
         <v/>
       </c>
       <c r="B114" t="s">
-        <v>246</v>
+        <v>406</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>245</v>
+        <v>403</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -8364,7 +8368,7 @@
         <v/>
       </c>
       <c r="B115" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>724</v>
@@ -8379,7 +8383,7 @@
         <v/>
       </c>
       <c r="B116" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>724</v>
@@ -8400,7 +8404,7 @@
         <v>724</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>396</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -8409,13 +8413,13 @@
         <v/>
       </c>
       <c r="B118" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>332</v>
+        <v>396</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -8424,13 +8428,13 @@
         <v/>
       </c>
       <c r="B119" t="s">
-        <v>407</v>
+        <v>331</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>408</v>
+        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -8439,13 +8443,13 @@
         <v/>
       </c>
       <c r="B120" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -8454,13 +8458,13 @@
         <v/>
       </c>
       <c r="B121" t="s">
-        <v>288</v>
+        <v>409</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>279</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -8469,13 +8473,13 @@
         <v/>
       </c>
       <c r="B122" t="s">
-        <v>333</v>
+        <v>288</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D122" t="s">
-        <v>761</v>
+      <c r="D122" s="4" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -8484,13 +8488,13 @@
         <v/>
       </c>
       <c r="B123" t="s">
-        <v>363</v>
+        <v>333</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D123" s="4" t="s">
-        <v>393</v>
+      <c r="D123" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -8504,8 +8508,8 @@
       <c r="C124" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D124" t="s">
-        <v>764</v>
+      <c r="D124" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -8514,13 +8518,13 @@
         <v/>
       </c>
       <c r="B125" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="C125" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D125" s="4" t="s">
-        <v>393</v>
+      <c r="D125" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -8529,13 +8533,13 @@
         <v/>
       </c>
       <c r="B126" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="C126" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -8544,13 +8548,13 @@
         <v/>
       </c>
       <c r="B127" t="s">
-        <v>270</v>
+        <v>411</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>271</v>
+        <v>412</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -8559,7 +8563,7 @@
         <v/>
       </c>
       <c r="B128" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>724</v>
@@ -8574,7 +8578,7 @@
         <v/>
       </c>
       <c r="B129" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>724</v>
@@ -8589,13 +8593,13 @@
         <v/>
       </c>
       <c r="B130" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>245</v>
+        <v>271</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -8604,13 +8608,13 @@
         <v/>
       </c>
       <c r="B131" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -8625,37 +8629,37 @@
         <v>724</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="str">
         <f>IF(ISNA(VLOOKUP(B133,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>738</v>
+      <c r="B133" t="s">
+        <v>261</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D133" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D133" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" t="str">
         <f>IF(ISNA(VLOOKUP(B134,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B134" t="s">
-        <v>289</v>
+      <c r="B134" s="2" t="s">
+        <v>738</v>
       </c>
       <c r="C134" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D134" s="4" t="s">
-        <v>279</v>
+      <c r="D134" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -8664,7 +8668,7 @@
         <v/>
       </c>
       <c r="B135" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>724</v>
@@ -8679,7 +8683,7 @@
         <v/>
       </c>
       <c r="B136" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>724</v>
@@ -8688,94 +8692,94 @@
         <v>279</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="str">
         <f>IF(ISNA(VLOOKUP(B137,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>344</v>
+      <c r="B137" t="s">
+        <v>291</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D137" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D137" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" t="str">
         <f>IF(ISNA(VLOOKUP(B138,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="2" t="s">
         <v>344</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D138" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D138" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="str">
         <f>IF(ISNA(VLOOKUP(B139,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>345</v>
+      <c r="B139" t="s">
+        <v>344</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D139" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D139" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" t="str">
         <f>IF(ISNA(VLOOKUP(B140,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="2" t="s">
         <v>345</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D140" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D140" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="str">
         <f>IF(ISNA(VLOOKUP(B141,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>346</v>
+      <c r="B141" t="s">
+        <v>345</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D141" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D141" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" t="str">
         <f>IF(ISNA(VLOOKUP(B142,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="2" t="s">
         <v>346</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D142" s="4" t="s">
-        <v>335</v>
+      <c r="D142" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -8784,13 +8788,13 @@
         <v/>
       </c>
       <c r="B143" t="s">
-        <v>314</v>
+        <v>346</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -8805,37 +8809,37 @@
         <v>724</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="str">
         <f>IF(ISNA(VLOOKUP(B145,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>348</v>
+      <c r="B145" t="s">
+        <v>314</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D145" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D145" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="str">
         <f>IF(ISNA(VLOOKUP(B146,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="2" t="s">
         <v>348</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D146" t="s">
-        <v>349</v>
+        <v>276</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -8844,13 +8848,13 @@
         <v/>
       </c>
       <c r="B147" t="s">
-        <v>250</v>
+        <v>348</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D147" s="4" t="s">
-        <v>245</v>
+      <c r="D147" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -8859,7 +8863,7 @@
         <v/>
       </c>
       <c r="B148" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>724</v>
@@ -8874,13 +8878,13 @@
         <v/>
       </c>
       <c r="B149" t="s">
-        <v>354</v>
+        <v>251</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>352</v>
+        <v>245</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -8889,13 +8893,13 @@
         <v/>
       </c>
       <c r="B150" t="s">
-        <v>395</v>
+        <v>354</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>393</v>
+        <v>352</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -8904,13 +8908,13 @@
         <v/>
       </c>
       <c r="B151" t="s">
-        <v>292</v>
+        <v>395</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D151" s="4" t="s">
-        <v>279</v>
+        <v>393</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -8925,7 +8929,7 @@
         <v>724</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>355</v>
+        <v>279</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -8934,13 +8938,13 @@
         <v/>
       </c>
       <c r="B153" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>279</v>
+        <v>355</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -8949,13 +8953,13 @@
         <v/>
       </c>
       <c r="B154" t="s">
-        <v>381</v>
+        <v>293</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>373</v>
+        <v>279</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -8964,7 +8968,7 @@
         <v/>
       </c>
       <c r="B155" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>724</v>
@@ -8979,7 +8983,7 @@
         <v/>
       </c>
       <c r="B156" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>724</v>
@@ -8994,13 +8998,13 @@
         <v/>
       </c>
       <c r="B157" t="s">
-        <v>262</v>
+        <v>383</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>258</v>
+        <v>373</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -9009,13 +9013,13 @@
         <v/>
       </c>
       <c r="B158" t="s">
-        <v>415</v>
+        <v>262</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>414</v>
+        <v>258</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -9024,13 +9028,13 @@
         <v/>
       </c>
       <c r="B159" t="s">
-        <v>263</v>
+        <v>415</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>258</v>
+        <v>414</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -9039,13 +9043,13 @@
         <v/>
       </c>
       <c r="B160" t="s">
-        <v>365</v>
+        <v>263</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>364</v>
+        <v>258</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -9054,13 +9058,13 @@
         <v/>
       </c>
       <c r="B161" t="s">
-        <v>274</v>
+        <v>365</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>271</v>
+        <v>364</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -9074,8 +9078,8 @@
       <c r="C162" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D162" t="s">
-        <v>766</v>
+      <c r="D162" s="4" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -9084,13 +9088,13 @@
         <v/>
       </c>
       <c r="B163" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D163" s="4" t="s">
-        <v>326</v>
+      <c r="D163" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -9099,13 +9103,13 @@
         <v/>
       </c>
       <c r="B164" t="s">
-        <v>366</v>
+        <v>325</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D164" t="s">
-        <v>767</v>
+      <c r="D164" s="4" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -9114,13 +9118,13 @@
         <v/>
       </c>
       <c r="B165" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D165" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -9129,13 +9133,13 @@
         <v/>
       </c>
       <c r="B166" t="s">
-        <v>309</v>
+        <v>367</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D166" s="4" t="s">
-        <v>310</v>
+      <c r="D166" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -9150,7 +9154,7 @@
         <v>724</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -9165,7 +9169,7 @@
         <v>724</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>393</v>
+        <v>327</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -9174,13 +9178,13 @@
         <v/>
       </c>
       <c r="B169" t="s">
-        <v>416</v>
+        <v>309</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D169" t="s">
-        <v>417</v>
+      <c r="D169" s="4" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.2">
@@ -9189,13 +9193,13 @@
         <v/>
       </c>
       <c r="B170" t="s">
-        <v>322</v>
+        <v>416</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D170" s="4" t="s">
-        <v>350</v>
+      <c r="D170" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -9210,7 +9214,7 @@
         <v>724</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -9224,8 +9228,8 @@
       <c r="C172" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D172" t="s">
-        <v>770</v>
+      <c r="D172" s="4" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -9240,7 +9244,7 @@
         <v>724</v>
       </c>
       <c r="D173" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -9254,8 +9258,8 @@
       <c r="C174" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D174" s="4" t="s">
-        <v>772</v>
+      <c r="D174" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -9264,13 +9268,13 @@
         <v/>
       </c>
       <c r="B175" t="s">
-        <v>294</v>
+        <v>322</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>279</v>
+        <v>772</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -9285,7 +9289,7 @@
         <v>724</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -9300,7 +9304,7 @@
         <v>724</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -9315,7 +9319,7 @@
         <v>724</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -9330,7 +9334,7 @@
         <v>724</v>
       </c>
       <c r="D179" s="4" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -9344,8 +9348,8 @@
       <c r="C180" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D180" t="s">
-        <v>770</v>
+      <c r="D180" s="4" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -9360,7 +9364,7 @@
         <v>724</v>
       </c>
       <c r="D181" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -9374,8 +9378,8 @@
       <c r="C182" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D182" s="4" t="s">
-        <v>772</v>
+      <c r="D182" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -9384,13 +9388,13 @@
         <v/>
       </c>
       <c r="B183" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>279</v>
+        <v>772</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -9405,7 +9409,7 @@
         <v>724</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -9420,7 +9424,7 @@
         <v>724</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -9435,7 +9439,7 @@
         <v>724</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -9450,7 +9454,7 @@
         <v>724</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.2">
@@ -9464,8 +9468,8 @@
       <c r="C188" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D188" t="s">
-        <v>770</v>
+      <c r="D188" s="4" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -9480,7 +9484,7 @@
         <v>724</v>
       </c>
       <c r="D189" t="s">
-        <v>764</v>
+        <v>770</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -9494,68 +9498,68 @@
       <c r="C190" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D190" s="4" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D190" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="str">
         <f>IF(ISNA(VLOOKUP(B191,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>735</v>
+      <c r="B191" t="s">
+        <v>295</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D191" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D191" s="4" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" t="str">
         <f>IF(ISNA(VLOOKUP(B192,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B192" t="s">
-        <v>368</v>
+      <c r="B192" s="2" t="s">
+        <v>735</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D192" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="str">
         <f>IF(ISNA(VLOOKUP(B193,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>418</v>
+      <c r="B193" t="s">
+        <v>368</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D193" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A194" t="str">
         <f>IF(ISNA(VLOOKUP(B194,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="2" t="s">
         <v>418</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D194" s="4" t="s">
-        <v>419</v>
+      <c r="D194" t="s">
+        <v>759</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -9564,13 +9568,13 @@
         <v/>
       </c>
       <c r="B195" t="s">
-        <v>252</v>
+        <v>418</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>245</v>
+        <v>419</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -9579,7 +9583,7 @@
         <v/>
       </c>
       <c r="B196" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>724</v>
@@ -9594,13 +9598,13 @@
         <v/>
       </c>
       <c r="B197" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D197" t="s">
-        <v>747</v>
+      <c r="D197" s="4" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -9609,13 +9613,13 @@
         <v/>
       </c>
       <c r="B198" t="s">
-        <v>384</v>
+        <v>241</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D198" s="4" t="s">
-        <v>373</v>
+      <c r="D198" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -9624,13 +9628,13 @@
         <v/>
       </c>
       <c r="B199" t="s">
-        <v>420</v>
+        <v>384</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>421</v>
+        <v>373</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -9639,13 +9643,13 @@
         <v/>
       </c>
       <c r="B200" t="s">
-        <v>385</v>
+        <v>420</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -9654,13 +9658,13 @@
         <v/>
       </c>
       <c r="B201" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D201" t="s">
-        <v>771</v>
+      <c r="D201" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -9669,13 +9673,13 @@
         <v/>
       </c>
       <c r="B202" t="s">
-        <v>296</v>
+        <v>391</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D202" s="4" t="s">
-        <v>279</v>
+      <c r="D202" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -9684,13 +9688,13 @@
         <v/>
       </c>
       <c r="B203" t="s">
-        <v>369</v>
+        <v>296</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>370</v>
+        <v>279</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -9699,7 +9703,7 @@
         <v/>
       </c>
       <c r="B204" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>724</v>
@@ -9714,7 +9718,7 @@
         <v/>
       </c>
       <c r="B205" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>724</v>
@@ -9729,13 +9733,13 @@
         <v/>
       </c>
       <c r="B206" t="s">
-        <v>315</v>
+        <v>372</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D206" s="4" t="s">
-        <v>313</v>
+        <v>370</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -9744,13 +9748,13 @@
         <v/>
       </c>
       <c r="B207" t="s">
-        <v>422</v>
+        <v>315</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>423</v>
+        <v>313</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -9759,7 +9763,7 @@
         <v/>
       </c>
       <c r="B208" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>724</v>
@@ -9774,13 +9778,13 @@
         <v/>
       </c>
       <c r="B209" t="s">
-        <v>356</v>
+        <v>424</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>355</v>
+        <v>423</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
@@ -9789,13 +9793,13 @@
         <v/>
       </c>
       <c r="B210" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D210" s="4" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -9804,13 +9808,13 @@
         <v/>
       </c>
       <c r="B211" t="s">
-        <v>242</v>
+        <v>386</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D211" t="s">
-        <v>749</v>
+      <c r="D211" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -9819,13 +9823,13 @@
         <v/>
       </c>
       <c r="B212" t="s">
-        <v>297</v>
+        <v>242</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D212" s="4" t="s">
-        <v>279</v>
+      <c r="D212" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
@@ -9834,13 +9838,13 @@
         <v/>
       </c>
       <c r="B213" t="s">
-        <v>25</v>
+        <v>297</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>373</v>
+        <v>279</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -9849,7 +9853,7 @@
         <v/>
       </c>
       <c r="B214" t="s">
-        <v>387</v>
+        <v>25</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>724</v>
@@ -9864,7 +9868,7 @@
         <v/>
       </c>
       <c r="B215" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>724</v>
@@ -9879,13 +9883,13 @@
         <v/>
       </c>
       <c r="B216" t="s">
-        <v>357</v>
+        <v>388</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D216" s="4" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -9894,13 +9898,13 @@
         <v/>
       </c>
       <c r="B217" t="s">
-        <v>298</v>
+        <v>357</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D217" s="4" t="s">
-        <v>279</v>
+        <v>355</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
@@ -9915,7 +9919,7 @@
         <v>724</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -9924,13 +9928,13 @@
         <v/>
       </c>
       <c r="B219" t="s">
-        <v>347</v>
+        <v>298</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -9939,13 +9943,13 @@
         <v/>
       </c>
       <c r="B220" t="s">
-        <v>254</v>
+        <v>347</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>245</v>
+        <v>335</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -9954,13 +9958,13 @@
         <v/>
       </c>
       <c r="B221" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -9969,13 +9973,13 @@
         <v/>
       </c>
       <c r="B222" t="s">
-        <v>255</v>
+        <v>299</v>
       </c>
       <c r="C222" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -9984,13 +9988,13 @@
         <v/>
       </c>
       <c r="B223" t="s">
-        <v>428</v>
+        <v>255</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>429</v>
+        <v>245</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -9999,13 +10003,13 @@
         <v/>
       </c>
       <c r="B224" t="s">
-        <v>305</v>
+        <v>428</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>302</v>
+        <v>429</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -10020,7 +10024,7 @@
         <v>724</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -10035,7 +10039,7 @@
         <v>724</v>
       </c>
       <c r="D226" s="4" t="s">
-        <v>373</v>
+        <v>311</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -10050,7 +10054,7 @@
         <v>724</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -10059,43 +10063,43 @@
         <v/>
       </c>
       <c r="B228" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D228" s="4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" t="str">
         <f>IF(ISNA(VLOOKUP(B229,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B229" s="2" t="s">
-        <v>726</v>
+      <c r="B229" t="s">
+        <v>318</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D229" s="4" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" t="str">
         <f>IF(ISNA(VLOOKUP(B230,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B230" t="s">
-        <v>358</v>
+      <c r="B230" s="2" t="s">
+        <v>726</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D230" s="4" t="s">
-        <v>355</v>
+        <v>725</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -10104,43 +10108,43 @@
         <v/>
       </c>
       <c r="B231" t="s">
-        <v>389</v>
+        <v>358</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D231" s="4" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" t="str">
         <f>IF(ISNA(VLOOKUP(B232,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B232" s="2" t="s">
-        <v>728</v>
+      <c r="B232" t="s">
+        <v>389</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" t="str">
         <f>IF(ISNA(VLOOKUP(B233,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B233" t="s">
-        <v>359</v>
+      <c r="B233" s="2" t="s">
+        <v>728</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>355</v>
+        <v>725</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -10149,25 +10153,28 @@
         <v/>
       </c>
       <c r="B234" t="s">
-        <v>390</v>
+        <v>359</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" t="str">
         <f>IF(ISNA(VLOOKUP(B235,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
+        <v/>
+      </c>
+      <c r="B235" t="s">
+        <v>390</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>724</v>
       </c>
-      <c r="D235" s="11" t="s">
-        <v>275</v>
+      <c r="D235" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -10175,12 +10182,11 @@
         <f>IF(ISNA(VLOOKUP(B236,Definitions!B$2:B$1638,1,FALSE)),"Not listed","")</f>
         <v>Not listed</v>
       </c>
-      <c r="B236" s="2"/>
       <c r="C236" s="4" t="s">
         <v>724</v>
       </c>
       <c r="D236" s="11" t="s">
-        <v>748</v>
+        <v>275</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added diggs_geo to LabCompactionTest
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rcutts/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1624D-6EC3-4846-BCA4-C36253E28461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4057C95-0C22-DF4A-AACE-96B872186F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1720" yWindow="500" windowWidth="35840" windowHeight="19900" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2375" uniqueCount="843">
   <si>
     <t>Description</t>
   </si>
@@ -2785,7 +2785,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2861,9 +2861,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3073,7 +3070,7 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Start" dataDxfId="12">
-      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3044,1,FALSE)),"Not used","")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3045,1,FALSE)),"Not used","")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ID" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Name" dataDxfId="10"/>
@@ -3088,10 +3085,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D430" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:D430" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D416">
-    <sortCondition ref="B1:B416"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D431" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:D431" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D417">
+    <sortCondition ref="B1:B417"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Start" dataDxfId="3">
@@ -3453,7 +3450,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A102" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
@@ -3498,7 +3495,7 @@
     </row>
     <row r="2" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3044,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B2,AssociatedElements!B$2:B3045,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B2" s="12" t="s">
@@ -3519,7 +3516,7 @@
     </row>
     <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B3213,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B3,AssociatedElements!B$2:B3214,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B3" s="2" t="s">
@@ -3537,7 +3534,7 @@
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B3210,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B4,AssociatedElements!B$2:B3211,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B4" s="2" t="s">
@@ -3555,7 +3552,7 @@
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B3045,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B5,AssociatedElements!B$2:B3046,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B5" s="2" t="s">
@@ -3576,7 +3573,7 @@
     </row>
     <row r="6" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B3046,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B6,AssociatedElements!B$2:B3047,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B6" s="2" t="s">
@@ -3597,7 +3594,7 @@
     </row>
     <row r="7" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B3047,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B7,AssociatedElements!B$2:B3048,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B7" s="2" t="s">
@@ -3618,7 +3615,7 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B3048,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B8,AssociatedElements!B$2:B3049,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B8" s="2" t="s">
@@ -3639,7 +3636,7 @@
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B3049,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B9,AssociatedElements!B$2:B3050,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B9" s="13" t="s">
@@ -3660,7 +3657,7 @@
     </row>
     <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B3050,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B10,AssociatedElements!B$2:B3051,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B10" s="13" t="s">
@@ -3681,7 +3678,7 @@
     </row>
     <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B3051,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B11,AssociatedElements!B$2:B3052,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B11" s="13" t="s">
@@ -3702,7 +3699,7 @@
     </row>
     <row r="12" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B3052,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B12,AssociatedElements!B$2:B3053,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B12" s="13" t="s">
@@ -3725,7 +3722,7 @@
     </row>
     <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B3053,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B13,AssociatedElements!B$2:B3054,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B13" s="13" t="s">
@@ -3748,7 +3745,7 @@
     </row>
     <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B3202,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B14,AssociatedElements!B$2:B3203,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B14" s="2" t="s">
@@ -3769,7 +3766,7 @@
     </row>
     <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B3054,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B15,AssociatedElements!B$2:B3055,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B15" s="13" t="s">
@@ -3792,7 +3789,7 @@
     </row>
     <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B3055,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B16,AssociatedElements!B$2:B3056,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B16" s="13" t="s">
@@ -3815,7 +3812,7 @@
     </row>
     <row r="17" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B3056,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B17,AssociatedElements!B$2:B3057,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B17" s="13" t="s">
@@ -3838,7 +3835,7 @@
     </row>
     <row r="18" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B3059,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B18,AssociatedElements!B$2:B3060,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B18" s="13" t="s">
@@ -3861,7 +3858,7 @@
     </row>
     <row r="19" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B3057,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B19,AssociatedElements!B$2:B3058,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B19" s="13" t="s">
@@ -3884,7 +3881,7 @@
     </row>
     <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B3058,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B20,AssociatedElements!B$2:B3059,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B20" s="13" t="s">
@@ -3907,7 +3904,7 @@
     </row>
     <row r="21" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B3059,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B21,AssociatedElements!B$2:B3060,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B21" s="13" t="s">
@@ -3930,7 +3927,7 @@
     </row>
     <row r="22" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B3060,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B22,AssociatedElements!B$2:B3061,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B22" s="13" t="s">
@@ -3953,7 +3950,7 @@
     </row>
     <row r="23" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B3061,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B23,AssociatedElements!B$2:B3062,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B23" s="13" t="s">
@@ -3976,7 +3973,7 @@
     </row>
     <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B3062,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B24,AssociatedElements!B$2:B3063,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B24" s="13" t="s">
@@ -3999,7 +3996,7 @@
     </row>
     <row r="25" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B3063,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B25,AssociatedElements!B$2:B3064,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B25" s="13" t="s">
@@ -4022,7 +4019,7 @@
     </row>
     <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B3064,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B26,AssociatedElements!B$2:B3065,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B26" s="13" t="s">
@@ -4045,7 +4042,7 @@
     </row>
     <row r="27" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B3065,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B27,AssociatedElements!B$2:B3066,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B27" s="13" t="s">
@@ -4068,7 +4065,7 @@
     </row>
     <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B3066,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B28,AssociatedElements!B$2:B3067,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B28" s="13" t="s">
@@ -4091,7 +4088,7 @@
     </row>
     <row r="29" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B3067,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B29,AssociatedElements!B$2:B3068,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B29" s="13" t="s">
@@ -4114,7 +4111,7 @@
     </row>
     <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B3068,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B30,AssociatedElements!B$2:B3069,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B30" s="13" t="s">
@@ -4137,7 +4134,7 @@
     </row>
     <row r="31" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B3069,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B31,AssociatedElements!B$2:B3070,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B31" s="13" t="s">
@@ -4160,7 +4157,7 @@
     </row>
     <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B3070,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B32,AssociatedElements!B$2:B3071,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B32" s="13" t="s">
@@ -4183,7 +4180,7 @@
     </row>
     <row r="33" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B3071,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B33,AssociatedElements!B$2:B3072,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B33" s="13" t="s">
@@ -4206,7 +4203,7 @@
     </row>
     <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B3072,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B34,AssociatedElements!B$2:B3073,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B34" s="13" t="s">
@@ -4229,7 +4226,7 @@
     </row>
     <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B3073,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B35,AssociatedElements!B$2:B3074,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B35" s="13" t="s">
@@ -4250,7 +4247,7 @@
     </row>
     <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B3074,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B36,AssociatedElements!B$2:B3075,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B36" s="13" t="s">
@@ -4271,7 +4268,7 @@
     </row>
     <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B3075,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B37,AssociatedElements!B$2:B3076,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B37" s="13" t="s">
@@ -4292,7 +4289,7 @@
     </row>
     <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B3076,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B38,AssociatedElements!B$2:B3077,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B38" s="13" t="s">
@@ -4313,7 +4310,7 @@
     </row>
     <row r="39" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B3077,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B39,AssociatedElements!B$2:B3078,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B39" s="13" t="s">
@@ -4334,7 +4331,7 @@
     </row>
     <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B3078,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B40,AssociatedElements!B$2:B3079,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B40" s="13" t="s">
@@ -4355,7 +4352,7 @@
     </row>
     <row r="41" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B3079,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B41,AssociatedElements!B$2:B3080,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B41" s="13" t="s">
@@ -4376,7 +4373,7 @@
     </row>
     <row r="42" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B3080,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B42,AssociatedElements!B$2:B3081,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B42" s="13" t="s">
@@ -4397,7 +4394,7 @@
     </row>
     <row r="43" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B3081,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B43,AssociatedElements!B$2:B3082,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B43" s="13" t="s">
@@ -4418,7 +4415,7 @@
     </row>
     <row r="44" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B3082,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B44,AssociatedElements!B$2:B3083,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B44" s="13" t="s">
@@ -4439,7 +4436,7 @@
     </row>
     <row r="45" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B45,AssociatedElements!B$2:B3207,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B45,AssociatedElements!B$2:B3208,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B45" s="13" t="s">
@@ -4460,7 +4457,7 @@
     </row>
     <row r="46" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B46,AssociatedElements!B$2:B3083,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B46,AssociatedElements!B$2:B3084,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B46" s="13" t="s">
@@ -4481,7 +4478,7 @@
     </row>
     <row r="47" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B47,AssociatedElements!B$2:B3084,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B47,AssociatedElements!B$2:B3085,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B47" s="13" t="s">
@@ -4502,7 +4499,7 @@
     </row>
     <row r="48" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B48,AssociatedElements!B$2:B3085,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B48,AssociatedElements!B$2:B3086,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B48" s="13" t="s">
@@ -4523,7 +4520,7 @@
     </row>
     <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B49,AssociatedElements!B$2:B3208,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B49,AssociatedElements!B$2:B3209,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B49" s="13" t="s">
@@ -4544,7 +4541,7 @@
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B50,AssociatedElements!B$2:B3086,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B50,AssociatedElements!B$2:B3087,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B50" s="13" t="s">
@@ -4565,7 +4562,7 @@
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B51,AssociatedElements!B$2:B3089,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B51,AssociatedElements!B$2:B3090,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B51" s="13" t="s">
@@ -4586,7 +4583,7 @@
     </row>
     <row r="52" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B52,AssociatedElements!B$2:B3087,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B52,AssociatedElements!B$2:B3088,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B52" s="13" t="s">
@@ -4607,7 +4604,7 @@
     </row>
     <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B53,AssociatedElements!B$2:B3088,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B53,AssociatedElements!B$2:B3089,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B53" s="13" t="s">
@@ -4628,7 +4625,7 @@
     </row>
     <row r="54" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B54,AssociatedElements!B$2:B3089,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B54,AssociatedElements!B$2:B3090,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B54" s="13" t="s">
@@ -4649,7 +4646,7 @@
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B55,AssociatedElements!B$2:B3090,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B55,AssociatedElements!B$2:B3091,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B55" s="13" t="s">
@@ -4670,7 +4667,7 @@
     </row>
     <row r="56" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B56,AssociatedElements!B$2:B3091,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B56,AssociatedElements!B$2:B3092,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B56" s="13" t="s">
@@ -4691,7 +4688,7 @@
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B57,AssociatedElements!B$2:B3092,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B57,AssociatedElements!B$2:B3093,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B57" s="13" t="s">
@@ -4712,7 +4709,7 @@
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B58,AssociatedElements!B$2:B3093,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B58,AssociatedElements!B$2:B3094,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B58" s="13" t="s">
@@ -4733,7 +4730,7 @@
     </row>
     <row r="59" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B59,AssociatedElements!B$2:B3094,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B59,AssociatedElements!B$2:B3095,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B59" s="13" t="s">
@@ -4754,7 +4751,7 @@
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B60,AssociatedElements!B$2:B3095,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B60,AssociatedElements!B$2:B3096,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B60" s="13" t="s">
@@ -4775,7 +4772,7 @@
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B61,AssociatedElements!B$2:B3096,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B61,AssociatedElements!B$2:B3097,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B61" s="13" t="s">
@@ -4796,7 +4793,7 @@
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B62,AssociatedElements!B$2:B3097,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B62,AssociatedElements!B$2:B3098,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B62" s="13" t="s">
@@ -4817,7 +4814,7 @@
     </row>
     <row r="63" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B63,AssociatedElements!B$2:B3098,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B63,AssociatedElements!B$2:B3099,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B63" s="13" t="s">
@@ -4838,7 +4835,7 @@
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B64,AssociatedElements!B$2:B3099,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B64,AssociatedElements!B$2:B3100,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B64" s="13" t="s">
@@ -4859,7 +4856,7 @@
     </row>
     <row r="65" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B65,AssociatedElements!B$2:B3100,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B65,AssociatedElements!B$2:B3101,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B65" s="13" t="s">
@@ -4880,7 +4877,7 @@
     </row>
     <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B66,AssociatedElements!B$2:B3101,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B66,AssociatedElements!B$2:B3102,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B66" s="13" t="s">
@@ -4901,7 +4898,7 @@
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B67,AssociatedElements!B$2:B3102,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B67,AssociatedElements!B$2:B3103,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B67" s="13" t="s">
@@ -4922,7 +4919,7 @@
     </row>
     <row r="68" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B68,AssociatedElements!B$2:B3103,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B68,AssociatedElements!B$2:B3104,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B68" s="13" t="s">
@@ -4943,7 +4940,7 @@
     </row>
     <row r="69" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B69,AssociatedElements!B$2:B3104,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B69,AssociatedElements!B$2:B3105,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B69" s="13" t="s">
@@ -4964,7 +4961,7 @@
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B70,AssociatedElements!B$2:B3105,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B70,AssociatedElements!B$2:B3106,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B70" s="13" t="s">
@@ -4985,7 +4982,7 @@
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B71,AssociatedElements!B$2:B3106,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B71,AssociatedElements!B$2:B3107,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B71" s="13" t="s">
@@ -5006,7 +5003,7 @@
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B72,AssociatedElements!B$2:B3107,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B72,AssociatedElements!B$2:B3108,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B72" s="13" t="s">
@@ -5027,7 +5024,7 @@
     </row>
     <row r="73" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B73,AssociatedElements!B$2:B3108,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B73,AssociatedElements!B$2:B3109,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B73" s="13" t="s">
@@ -5048,7 +5045,7 @@
     </row>
     <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B74,AssociatedElements!B$2:B3109,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B74,AssociatedElements!B$2:B3110,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B74" s="13" t="s">
@@ -5069,7 +5066,7 @@
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B75,AssociatedElements!B$2:B3110,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B75,AssociatedElements!B$2:B3111,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B75" s="13" t="s">
@@ -5090,7 +5087,7 @@
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B76,AssociatedElements!B$2:B3111,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B76,AssociatedElements!B$2:B3112,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B76" s="13" t="s">
@@ -5111,7 +5108,7 @@
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B77,AssociatedElements!B$2:B3112,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B77,AssociatedElements!B$2:B3113,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B77" s="13" t="s">
@@ -5132,7 +5129,7 @@
     </row>
     <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B78,AssociatedElements!B$2:B3113,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B78,AssociatedElements!B$2:B3114,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B78" s="13" t="s">
@@ -5153,7 +5150,7 @@
     </row>
     <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B79,AssociatedElements!B$2:B3114,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B79,AssociatedElements!B$2:B3115,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B79" s="13" t="s">
@@ -5174,7 +5171,7 @@
     </row>
     <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B80,AssociatedElements!B$2:B3115,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B80,AssociatedElements!B$2:B3116,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B80" s="13" t="s">
@@ -5195,7 +5192,7 @@
     </row>
     <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B81,AssociatedElements!B$2:B3116,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B81,AssociatedElements!B$2:B3117,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B81" s="13" t="s">
@@ -5216,7 +5213,7 @@
     </row>
     <row r="82" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B82,AssociatedElements!B$2:B3117,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B82,AssociatedElements!B$2:B3118,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B82" s="13" t="s">
@@ -5237,7 +5234,7 @@
     </row>
     <row r="83" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B83,AssociatedElements!B$2:B3118,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B83,AssociatedElements!B$2:B3119,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B83" s="13" t="s">
@@ -5258,7 +5255,7 @@
     </row>
     <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B84,AssociatedElements!B$2:B3119,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B84,AssociatedElements!B$2:B3120,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B84" s="13" t="s">
@@ -5279,7 +5276,7 @@
     </row>
     <row r="85" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B85,AssociatedElements!B$2:B3120,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B85,AssociatedElements!B$2:B3121,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B85" s="13" t="s">
@@ -5300,7 +5297,7 @@
     </row>
     <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B86,AssociatedElements!B$2:B3121,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B86,AssociatedElements!B$2:B3122,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B86" s="13" t="s">
@@ -5321,7 +5318,7 @@
     </row>
     <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B87,AssociatedElements!B$2:B3122,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B87,AssociatedElements!B$2:B3123,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B87" s="13" t="s">
@@ -5342,7 +5339,7 @@
     </row>
     <row r="88" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B88,AssociatedElements!B$2:B3123,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B88,AssociatedElements!B$2:B3124,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B88" s="13" t="s">
@@ -5363,7 +5360,7 @@
     </row>
     <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B89,AssociatedElements!B$2:B3124,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B89,AssociatedElements!B$2:B3125,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B89" s="13" t="s">
@@ -5384,7 +5381,7 @@
     </row>
     <row r="90" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B90,AssociatedElements!B$2:B3125,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B90,AssociatedElements!B$2:B3126,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B90" s="13" t="s">
@@ -5405,7 +5402,7 @@
     </row>
     <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B91,AssociatedElements!B$2:B3126,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B91,AssociatedElements!B$2:B3127,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B91" s="13" t="s">
@@ -5426,7 +5423,7 @@
     </row>
     <row r="92" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B92,AssociatedElements!B$2:B3127,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B92,AssociatedElements!B$2:B3128,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B92" s="13" t="s">
@@ -5447,7 +5444,7 @@
     </row>
     <row r="93" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B93,AssociatedElements!B$2:B3128,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B93,AssociatedElements!B$2:B3129,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B93" s="13" t="s">
@@ -5468,7 +5465,7 @@
     </row>
     <row r="94" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B94,AssociatedElements!B$2:B3129,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B94,AssociatedElements!B$2:B3130,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B94" s="13" t="s">
@@ -5489,7 +5486,7 @@
     </row>
     <row r="95" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B95,AssociatedElements!B$2:B3130,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B95,AssociatedElements!B$2:B3131,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B95" s="13" t="s">
@@ -5510,7 +5507,7 @@
     </row>
     <row r="96" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B96,AssociatedElements!B$2:B3131,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B96,AssociatedElements!B$2:B3132,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B96" s="13" t="s">
@@ -5531,7 +5528,7 @@
     </row>
     <row r="97" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B97,AssociatedElements!B$2:B3201,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B97,AssociatedElements!B$2:B3202,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B97" s="2" t="s">
@@ -5552,7 +5549,7 @@
     </row>
     <row r="98" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B98,AssociatedElements!B$2:B3132,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B98,AssociatedElements!B$2:B3133,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B98" s="13" t="s">
@@ -5573,7 +5570,7 @@
     </row>
     <row r="99" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B99,AssociatedElements!B$2:B3133,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B99,AssociatedElements!B$2:B3134,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B99" s="13" t="s">
@@ -5594,7 +5591,7 @@
     </row>
     <row r="100" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B100,AssociatedElements!B$2:B3134,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B100,AssociatedElements!B$2:B3135,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B100" s="13" t="s">
@@ -5615,7 +5612,7 @@
     </row>
     <row r="101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B101,AssociatedElements!B$2:B3138,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B101,AssociatedElements!B$2:B3139,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B101" s="19" t="s">
@@ -5637,7 +5634,7 @@
     </row>
     <row r="102" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B102,AssociatedElements!B$2:B3218,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B102,AssociatedElements!B$2:B3219,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B102" s="2" t="s">
@@ -5658,7 +5655,7 @@
     </row>
     <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B103,AssociatedElements!B$2:B3135,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B103,AssociatedElements!B$2:B3136,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B103" s="13" t="s">
@@ -5679,7 +5676,7 @@
     </row>
     <row r="104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B104,AssociatedElements!B$2:B3136,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B104,AssociatedElements!B$2:B3137,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B104" s="13" t="s">
@@ -5700,7 +5697,7 @@
     </row>
     <row r="105" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B105,AssociatedElements!B$2:B3137,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B105,AssociatedElements!B$2:B3138,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B105" s="13" t="s">
@@ -5721,7 +5718,7 @@
     </row>
     <row r="106" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B106,AssociatedElements!B$2:B3214,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B106,AssociatedElements!B$2:B3215,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B106" s="2" t="s">
@@ -5742,7 +5739,7 @@
     </row>
     <row r="107" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B107,AssociatedElements!B$2:B3138,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B107,AssociatedElements!B$2:B3139,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B107" s="13" t="s">
@@ -5763,7 +5760,7 @@
     </row>
     <row r="108" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B108,AssociatedElements!B$2:B3139,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B108,AssociatedElements!B$2:B3140,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B108" s="13" t="s">
@@ -5784,7 +5781,7 @@
     </row>
     <row r="109" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B109,AssociatedElements!B$2:B3140,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B109,AssociatedElements!B$2:B3141,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B109" s="13" t="s">
@@ -5805,7 +5802,7 @@
     </row>
     <row r="110" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B110,AssociatedElements!B$2:B3141,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B110,AssociatedElements!B$2:B3142,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B110" s="13" t="s">
@@ -5826,7 +5823,7 @@
     </row>
     <row r="111" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B111,AssociatedElements!B$2:B3142,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B111,AssociatedElements!B$2:B3143,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B111" s="13" t="s">
@@ -5847,7 +5844,7 @@
     </row>
     <row r="112" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B112,AssociatedElements!B$2:B3143,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B112,AssociatedElements!B$2:B3144,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B112" s="13" t="s">
@@ -5868,7 +5865,7 @@
     </row>
     <row r="113" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B113,AssociatedElements!B$2:B3144,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B113,AssociatedElements!B$2:B3145,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B113" s="13" t="s">
@@ -5889,7 +5886,7 @@
     </row>
     <row r="114" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B114,AssociatedElements!B$2:B3145,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B114,AssociatedElements!B$2:B3146,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B114" s="13" t="s">
@@ -5910,7 +5907,7 @@
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B115,AssociatedElements!B$2:B3146,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B115,AssociatedElements!B$2:B3147,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B115" s="13" t="s">
@@ -5931,7 +5928,7 @@
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B116,AssociatedElements!B$2:B3147,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B116,AssociatedElements!B$2:B3148,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B116" s="13" t="s">
@@ -5952,7 +5949,7 @@
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B117,AssociatedElements!B$2:B3148,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B117,AssociatedElements!B$2:B3149,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B117" s="13" t="s">
@@ -5973,7 +5970,7 @@
     </row>
     <row r="118" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B118,AssociatedElements!B$2:B3149,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B118,AssociatedElements!B$2:B3150,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B118" s="13" t="s">
@@ -5994,7 +5991,7 @@
     </row>
     <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B119,AssociatedElements!B$2:B3150,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B119,AssociatedElements!B$2:B3151,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B119" s="13" t="s">
@@ -6015,7 +6012,7 @@
     </row>
     <row r="120" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B120,AssociatedElements!B$2:B3151,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B120,AssociatedElements!B$2:B3152,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B120" s="13" t="s">
@@ -6036,7 +6033,7 @@
     </row>
     <row r="121" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B121,AssociatedElements!B$2:B3152,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B121,AssociatedElements!B$2:B3153,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B121" s="13" t="s">
@@ -6057,7 +6054,7 @@
     </row>
     <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B122,AssociatedElements!B$2:B3153,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B122,AssociatedElements!B$2:B3154,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B122" s="13" t="s">
@@ -6078,7 +6075,7 @@
     </row>
     <row r="123" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B123,AssociatedElements!B$2:B3154,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B123,AssociatedElements!B$2:B3155,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B123" s="13" t="s">
@@ -6099,7 +6096,7 @@
     </row>
     <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B124,AssociatedElements!B$2:B3155,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B124,AssociatedElements!B$2:B3156,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B124" s="13" t="s">
@@ -6120,7 +6117,7 @@
     </row>
     <row r="125" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B125,AssociatedElements!B$2:B3156,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B125,AssociatedElements!B$2:B3157,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B125" s="13" t="s">
@@ -6141,7 +6138,7 @@
     </row>
     <row r="126" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B126,AssociatedElements!B$2:B3157,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B126,AssociatedElements!B$2:B3158,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B126" s="13" t="s">
@@ -6162,7 +6159,7 @@
     </row>
     <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B127,AssociatedElements!B$2:B3158,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B127,AssociatedElements!B$2:B3159,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B127" s="13" t="s">
@@ -6183,7 +6180,7 @@
     </row>
     <row r="128" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B128,AssociatedElements!B$2:B3159,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B128,AssociatedElements!B$2:B3160,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B128" s="13" t="s">
@@ -6204,7 +6201,7 @@
     </row>
     <row r="129" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B129,AssociatedElements!B$2:B3160,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B129,AssociatedElements!B$2:B3161,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B129" s="13" t="s">
@@ -6225,7 +6222,7 @@
     </row>
     <row r="130" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B130,AssociatedElements!B$2:B3161,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B130,AssociatedElements!B$2:B3162,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B130" s="13" t="s">
@@ -6246,7 +6243,7 @@
     </row>
     <row r="131" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B131,AssociatedElements!B$2:B3200,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B131,AssociatedElements!B$2:B3201,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B131" s="2" t="s">
@@ -6267,7 +6264,7 @@
     </row>
     <row r="132" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B132,AssociatedElements!B$2:B3162,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B132,AssociatedElements!B$2:B3163,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B132" s="13" t="s">
@@ -6288,7 +6285,7 @@
     </row>
     <row r="133" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B133,AssociatedElements!B$2:B3163,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B133,AssociatedElements!B$2:B3164,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B133" s="13" t="s">
@@ -6309,7 +6306,7 @@
     </row>
     <row r="134" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B134,AssociatedElements!B$2:B3164,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B134,AssociatedElements!B$2:B3165,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B134" s="13" t="s">
@@ -6330,7 +6327,7 @@
     </row>
     <row r="135" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B135,AssociatedElements!B$2:B3165,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B135,AssociatedElements!B$2:B3166,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B135" s="13" t="s">
@@ -6351,7 +6348,7 @@
     </row>
     <row r="136" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B136,AssociatedElements!B$2:B3166,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B136,AssociatedElements!B$2:B3167,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B136" s="13" t="s">
@@ -6372,7 +6369,7 @@
     </row>
     <row r="137" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B137,AssociatedElements!B$2:B3167,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B137,AssociatedElements!B$2:B3168,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B137" s="13" t="s">
@@ -6393,7 +6390,7 @@
     </row>
     <row r="138" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B138,AssociatedElements!B$2:B3168,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B138,AssociatedElements!B$2:B3169,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B138" s="13" t="s">
@@ -6414,7 +6411,7 @@
     </row>
     <row r="139" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B139,AssociatedElements!B$2:B3169,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B139,AssociatedElements!B$2:B3170,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B139" s="13" t="s">
@@ -6435,7 +6432,7 @@
     </row>
     <row r="140" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B140,AssociatedElements!B$2:B3170,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B140,AssociatedElements!B$2:B3171,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B140" s="13" t="s">
@@ -6456,7 +6453,7 @@
     </row>
     <row r="141" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B141,AssociatedElements!B$2:B3171,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B141,AssociatedElements!B$2:B3172,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B141" s="13" t="s">
@@ -6475,7 +6472,7 @@
     </row>
     <row r="142" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B142,AssociatedElements!B$2:B3172,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B142,AssociatedElements!B$2:B3173,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B142" s="13" t="s">
@@ -6496,7 +6493,7 @@
     </row>
     <row r="143" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B143,AssociatedElements!B$2:B3173,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B143,AssociatedElements!B$2:B3174,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B143" s="13" t="s">
@@ -6517,7 +6514,7 @@
     </row>
     <row r="144" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B144,AssociatedElements!B$2:B3174,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B144,AssociatedElements!B$2:B3175,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B144" s="13" t="s">
@@ -6538,7 +6535,7 @@
     </row>
     <row r="145" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B145,AssociatedElements!B$2:B3175,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B145,AssociatedElements!B$2:B3176,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B145" s="13" t="s">
@@ -6559,7 +6556,7 @@
     </row>
     <row r="146" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B146,AssociatedElements!B$2:B3176,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B146,AssociatedElements!B$2:B3177,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B146" s="13" t="s">
@@ -6580,7 +6577,7 @@
     </row>
     <row r="147" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B147,AssociatedElements!B$2:B3177,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B147,AssociatedElements!B$2:B3178,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B147" s="13" t="s">
@@ -6601,7 +6598,7 @@
     </row>
     <row r="148" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B148,AssociatedElements!B$2:B3178,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B148,AssociatedElements!B$2:B3179,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B148" s="13" t="s">
@@ -6622,7 +6619,7 @@
     </row>
     <row r="149" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B149,AssociatedElements!B$2:B3179,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B149,AssociatedElements!B$2:B3180,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B149" s="13" t="s">
@@ -6643,7 +6640,7 @@
     </row>
     <row r="150" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B150,AssociatedElements!B$2:B3180,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B150,AssociatedElements!B$2:B3181,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B150" s="13" t="s">
@@ -6664,7 +6661,7 @@
     </row>
     <row r="151" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B151,AssociatedElements!B$2:B3181,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B151,AssociatedElements!B$2:B3182,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B151" s="13" t="s">
@@ -6685,7 +6682,7 @@
     </row>
     <row r="152" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B152,AssociatedElements!B$2:B3182,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B152,AssociatedElements!B$2:B3183,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B152" s="13" t="s">
@@ -6706,7 +6703,7 @@
     </row>
     <row r="153" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B153,AssociatedElements!B$2:B3183,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B153,AssociatedElements!B$2:B3184,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B153" s="13" t="s">
@@ -6727,7 +6724,7 @@
     </row>
     <row r="154" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B154,AssociatedElements!B$2:B3184,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B154,AssociatedElements!B$2:B3185,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B154" s="13" t="s">
@@ -6748,7 +6745,7 @@
     </row>
     <row r="155" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B155,AssociatedElements!B$2:B3206,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B155,AssociatedElements!B$2:B3207,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B155" s="2" t="s">
@@ -6769,7 +6766,7 @@
     </row>
     <row r="156" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B156,AssociatedElements!B$2:B3185,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B156,AssociatedElements!B$2:B3186,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B156" s="13" t="s">
@@ -6790,7 +6787,7 @@
     </row>
     <row r="157" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B157,AssociatedElements!B$2:B3186,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B157,AssociatedElements!B$2:B3187,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B157" s="13" t="s">
@@ -6811,7 +6808,7 @@
     </row>
     <row r="158" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B158,AssociatedElements!B$2:B3209,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B158,AssociatedElements!B$2:B3210,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B158" s="2" t="s">
@@ -6829,7 +6826,7 @@
     </row>
     <row r="159" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B159,AssociatedElements!B$2:B3187,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B159,AssociatedElements!B$2:B3188,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B159" s="13" t="s">
@@ -6848,7 +6845,7 @@
     </row>
     <row r="160" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B160,AssociatedElements!B$2:B3188,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B160,AssociatedElements!B$2:B3189,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B160" s="13" t="s">
@@ -6867,7 +6864,7 @@
     </row>
     <row r="161" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B161,AssociatedElements!B$2:B3189,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B161,AssociatedElements!B$2:B3190,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B161" s="13" t="s">
@@ -6888,7 +6885,7 @@
     </row>
     <row r="162" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B162,AssociatedElements!B$2:B3190,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B162,AssociatedElements!B$2:B3191,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B162" s="13" t="s">
@@ -6909,7 +6906,7 @@
     </row>
     <row r="163" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B163,AssociatedElements!B$2:B3191,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B163,AssociatedElements!B$2:B3192,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B163" s="13" t="s">
@@ -6928,7 +6925,7 @@
     </row>
     <row r="164" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B164,AssociatedElements!B$2:B3192,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B164,AssociatedElements!B$2:B3193,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B164" s="13" t="s">
@@ -6949,7 +6946,7 @@
     </row>
     <row r="165" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B165,AssociatedElements!B$2:B3193,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B165,AssociatedElements!B$2:B3194,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B165" s="13" t="s">
@@ -6970,7 +6967,7 @@
     </row>
     <row r="166" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B166,AssociatedElements!B$2:B3194,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B166,AssociatedElements!B$2:B3195,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B166" s="13" t="s">
@@ -6991,7 +6988,7 @@
     </row>
     <row r="167" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B167,AssociatedElements!B$2:B3194,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B167,AssociatedElements!B$2:B3195,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B167" s="13" t="s">
@@ -7012,7 +7009,7 @@
     </row>
     <row r="168" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B168,AssociatedElements!B$2:B3196,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B168,AssociatedElements!B$2:B3197,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B168" s="13" t="s">
@@ -7033,7 +7030,7 @@
     </row>
     <row r="169" spans="1:6" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B169,AssociatedElements!B$2:B3194,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B169,AssociatedElements!B$2:B3195,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B169" s="13" t="s">
@@ -7054,7 +7051,7 @@
     </row>
     <row r="170" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B170,AssociatedElements!B$2:B3195,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B170,AssociatedElements!B$2:B3196,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B170" s="13" t="s">
@@ -7075,7 +7072,7 @@
     </row>
     <row r="171" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="str">
-        <f>IF(ISNA(VLOOKUP(B171,AssociatedElements!B$2:B3197,1,FALSE)),"Not used","")</f>
+        <f>IF(ISNA(VLOOKUP(B171,AssociatedElements!B$2:B3198,1,FALSE)),"Not used","")</f>
         <v/>
       </c>
       <c r="B171" s="13" t="s">
@@ -7124,11 +7121,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D430"/>
+  <dimension ref="A1:D431"/>
   <sheetViews>
-    <sheetView zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A378" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D402" sqref="D402"/>
+    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A394" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C406" sqref="C406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13158,44 +13155,44 @@
         <f>IF(ISNA(VLOOKUP(B402,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B402" s="33" t="s">
+      <c r="B402" s="29" t="s">
         <v>297</v>
       </c>
       <c r="C402" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D402" s="24" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.2">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A403" t="str">
         <f>IF(ISNA(VLOOKUP(B403,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B403" t="s">
-        <v>306</v>
-      </c>
-      <c r="C403" s="4" t="s">
+      <c r="B403" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="C403" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D403" s="24" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="404" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A404" t="str">
         <f>IF(ISNA(VLOOKUP(B404,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B404" s="29" t="s">
+      <c r="B404" t="s">
         <v>306</v>
       </c>
-      <c r="C404" s="24" t="s">
+      <c r="C404" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D404" s="24" t="s">
-        <v>805</v>
+        <v>730</v>
       </c>
     </row>
     <row r="405" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13203,74 +13200,74 @@
         <f>IF(ISNA(VLOOKUP(B405,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B405" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="C405" s="4" t="s">
+      <c r="B405" s="29" t="s">
+        <v>306</v>
+      </c>
+      <c r="C405" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D405" s="24" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.2">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A406" t="str">
         <f>IF(ISNA(VLOOKUP(B406,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B406" t="s">
-        <v>336</v>
+      <c r="B406" s="2" t="s">
+        <v>668</v>
       </c>
       <c r="C406" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D406" s="24" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="407" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A407" t="str">
         <f>IF(ISNA(VLOOKUP(B407,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B407" s="29" t="s">
+      <c r="B407" t="s">
         <v>336</v>
       </c>
-      <c r="C407" s="24" t="s">
+      <c r="C407" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D407" s="24" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.2">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A408" t="str">
         <f>IF(ISNA(VLOOKUP(B408,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B408" t="s">
-        <v>364</v>
-      </c>
-      <c r="C408" s="4" t="s">
+      <c r="B408" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="C408" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D408" s="24" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="409" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A409" t="str">
         <f>IF(ISNA(VLOOKUP(B409,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B409" s="29" t="s">
+      <c r="B409" t="s">
         <v>364</v>
       </c>
-      <c r="C409" s="24" t="s">
+      <c r="C409" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D409" s="24" t="s">
-        <v>819</v>
+        <v>721</v>
       </c>
     </row>
     <row r="410" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13278,87 +13275,89 @@
         <f>IF(ISNA(VLOOKUP(B410,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B410" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="C410" s="4" t="s">
+      <c r="B410" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="C410" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D410" s="24" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.2">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A411" t="str">
         <f>IF(ISNA(VLOOKUP(B411,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B411" t="s">
-        <v>337</v>
+      <c r="B411" s="2" t="s">
+        <v>670</v>
       </c>
       <c r="C411" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D411" s="24" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="412" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A412" t="str">
         <f>IF(ISNA(VLOOKUP(B412,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B412" s="29" t="s">
+      <c r="B412" t="s">
         <v>337</v>
       </c>
-      <c r="C412" s="24" t="s">
+      <c r="C412" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D412" s="24" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A413" t="str">
         <f>IF(ISNA(VLOOKUP(B413,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B413" t="s">
-        <v>365</v>
-      </c>
-      <c r="C413" s="4" t="s">
+      <c r="B413" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="C413" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D413" s="24" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="414" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A414" t="str">
         <f>IF(ISNA(VLOOKUP(B414,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
         <v/>
       </c>
-      <c r="B414" s="29" t="s">
+      <c r="B414" t="s">
         <v>365</v>
       </c>
-      <c r="C414" s="24" t="s">
+      <c r="C414" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D414" s="24" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.2">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A415" t="str">
         <f>IF(ISNA(VLOOKUP(B415,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
-        <v>Not listed</v>
-      </c>
-      <c r="B415" s="2"/>
-      <c r="C415" s="4" t="s">
+        <v/>
+      </c>
+      <c r="B415" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="C415" s="24" t="s">
         <v>773</v>
       </c>
       <c r="D415" s="24" t="s">
-        <v>769</v>
+        <v>819</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.2">
@@ -13371,22 +13370,20 @@
         <v>773</v>
       </c>
       <c r="D416" s="24" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="417" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A417" t="str">
         <f>IF(ISNA(VLOOKUP(B417,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
-        <v/>
-      </c>
-      <c r="B417" s="2" t="s">
-        <v>822</v>
-      </c>
+        <v>Not listed</v>
+      </c>
+      <c r="B417" s="2"/>
       <c r="C417" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D417" s="24" t="s">
-        <v>715</v>
+        <v>772</v>
       </c>
     </row>
     <row r="418" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13401,7 +13398,7 @@
         <v>773</v>
       </c>
       <c r="D418" s="24" t="s">
-        <v>812</v>
+        <v>715</v>
       </c>
     </row>
     <row r="419" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13410,13 +13407,13 @@
         <v/>
       </c>
       <c r="B419" s="2" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="C419" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D419" s="24" t="s">
-        <v>715</v>
+        <v>812</v>
       </c>
     </row>
     <row r="420" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13431,7 +13428,7 @@
         <v>773</v>
       </c>
       <c r="D420" s="24" t="s">
-        <v>812</v>
+        <v>715</v>
       </c>
     </row>
     <row r="421" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13440,13 +13437,13 @@
         <v/>
       </c>
       <c r="B421" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C421" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D421" s="24" t="s">
-        <v>715</v>
+        <v>812</v>
       </c>
     </row>
     <row r="422" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13461,7 +13458,7 @@
         <v>773</v>
       </c>
       <c r="D422" s="24" t="s">
-        <v>812</v>
+        <v>715</v>
       </c>
     </row>
     <row r="423" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13470,13 +13467,13 @@
         <v/>
       </c>
       <c r="B423" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D423" s="24" t="s">
-        <v>718</v>
+        <v>812</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13491,7 +13488,7 @@
         <v>773</v>
       </c>
       <c r="D424" s="24" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="425" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13506,7 +13503,7 @@
         <v>773</v>
       </c>
       <c r="D425" s="24" t="s">
-        <v>811</v>
+        <v>715</v>
       </c>
     </row>
     <row r="426" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13521,7 +13518,7 @@
         <v>773</v>
       </c>
       <c r="D426" s="24" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="427" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13530,13 +13527,13 @@
         <v/>
       </c>
       <c r="B427" s="2" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>773</v>
       </c>
       <c r="D427" s="24" t="s">
-        <v>718</v>
+        <v>812</v>
       </c>
     </row>
     <row r="428" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13551,7 +13548,7 @@
         <v>773</v>
       </c>
       <c r="D428" s="24" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="429" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13566,7 +13563,7 @@
         <v>773</v>
       </c>
       <c r="D429" s="24" t="s">
-        <v>811</v>
+        <v>715</v>
       </c>
     </row>
     <row r="430" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13581,6 +13578,21 @@
         <v>773</v>
       </c>
       <c r="D430" s="24" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A431" t="str">
+        <f>IF(ISNA(VLOOKUP(B431,Definitions!B$2:B$1633,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B431" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="C431" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="D431" s="24" t="s">
         <v>812</v>
       </c>
     </row>
@@ -13602,7 +13614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update properties and roles excel dictionaries
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F496D6BE-53D9-3949-BA9D-12353070D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABEE333-03E9-8245-BAF5-C6F34A10D1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="2660" windowWidth="47440" windowHeight="28160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6140" yWindow="3060" windowWidth="47440" windowHeight="28160" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -7317,8 +7317,8 @@
   <dimension ref="A1:D295"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C283" sqref="C283"/>
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D280" sqref="D280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update properties.xls and validation modules
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B9E29B-7699-E345-AD46-6CEB3CE38C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F543F630-571C-854C-A086-BDA64C37D97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14420" yWindow="3740" windowWidth="41160" windowHeight="27020" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14420" yWindow="3740" windowWidth="41160" windowHeight="27020" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryName" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="841">
   <si>
     <t>Description</t>
   </si>
@@ -2560,6 +2560,9 @@
   </si>
   <si>
     <t>ancestor::SpatialResult</t>
+  </si>
+  <si>
+    <t>ancestor::diggs:measurement//diggs:procedure/diggs:FluidLevelMonitoring</t>
   </si>
 </sst>
 </file>
@@ -2805,7 +2808,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2889,6 +2892,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3113,7 +3124,7 @@
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4" refreshError="1"/>
     </sheetDataSet>
@@ -3158,8 +3169,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D273" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:D273" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="AssociatedElements" displayName="AssociatedElements" ref="A1:D276" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:D276" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D273">
     <sortCondition ref="C1:C273"/>
   </sortState>
@@ -3526,7 +3537,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -7265,11 +7276,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D273"/>
+  <dimension ref="A1:D276"/>
   <sheetViews>
-    <sheetView zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D244" sqref="D244"/>
+    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E277" sqref="E277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11368,6 +11379,51 @@
       </c>
       <c r="D273" s="24" t="s">
         <v>805</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A274" s="37" t="str">
+        <f>IF(ISNA(VLOOKUP([1]AssociatedElements!B274,Definitions!B$2:B$1623,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B274" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="C274" s="39" t="s">
+        <v>668</v>
+      </c>
+      <c r="D274" s="24" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A275" s="37" t="str">
+        <f>IF(ISNA(VLOOKUP([1]AssociatedElements!B275,Definitions!B$2:B$1623,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B275" s="38" t="s">
+        <v>644</v>
+      </c>
+      <c r="C275" s="39" t="s">
+        <v>668</v>
+      </c>
+      <c r="D275" s="24" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A276" s="37" t="str">
+        <f>IF(ISNA(VLOOKUP([1]AssociatedElements!B276,Definitions!B$2:B$1623,1,FALSE)),"Not listed","")</f>
+        <v/>
+      </c>
+      <c r="B276" s="40" t="s">
+        <v>345</v>
+      </c>
+      <c r="C276" s="39" t="s">
+        <v>668</v>
+      </c>
+      <c r="D276" s="24" t="s">
+        <v>840</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Diggs UOM Dictionary
</commit_message>
<xml_diff>
--- a/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
+++ b/Codelist Excel Files and Conversion Templates to XML/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dponti/GitHub/def/Codelist Excel Files and Conversion Templates to XML/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BBC905-294D-D54B-A226-1DE77A3B079B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67937E41-13FD-5645-BB73-C58DC456B0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3740" yWindow="1740" windowWidth="53300" windowHeight="29520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3694,8 +3694,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -5181,7 +5181,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>197</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="34">
@@ -12164,8 +12164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J188"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A123" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>